<commit_message>
enable the configuration of the library through appsettings.json.
</commit_message>
<xml_diff>
--- a/samples/1.json-sample-and-test.xlsx
+++ b/samples/1.json-sample-and-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\git\exlibris\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC41DE29-C2BF-4F4F-88EA-66CAD2599C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CC5CA1-F4E1-4215-B834-6F67F0C82B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34510" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{70191E0D-F6B7-49FF-9AAA-6C22F5510F3E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{70191E0D-F6B7-49FF-9AAA-6C22F5510F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="top" sheetId="1" r:id="rId1"/>
@@ -526,9 +526,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{"definitions":{"ExcelValueConversionConfiguration":{"type":["object","null"],"properties":{"excel_error_to":{"type":"integer","enum":["excel_error","null","string_empty"]},"excel_missing_to":{"type":"integer","enum":["excel_error","null","string_empty"]},"excel_empty_to":{"type":"integer","enum":["excel_error","null","string_empty"]},"excel_string_empty_to":{"type":"integer","enum":["excel_error","null","string_empty"]},"null_to":{"type":"integer","enum":["excel_empty","string_empty"]},"string_empty_to":{"type":"integer","enum":["excel_empty","string_empty"]}}}},"type":"object","properties":{"excel_value_conversion":{"$ref":"#/definitions/ExcelValueConversionConfiguration"}}}</t>
-  </si>
-  <si>
     <t>{"$schema":"http://json-schema.org/draft-07/schema#","$id":"http://example.com/product.schema.json","title":"Product","description":"A product from Acme's catalog","type":"object","additionalProperties":false,"properties":{"productId":{"description":"The unique identifier for a product","type":"integer"},"productName":{"description":"Name of the product","type":"string"},"price":{"description":"The price of the product","type":"number","exclusiveMinimum":0.0},"tags":{"description":"Tags for the product","type":"array","items":{"type":"string"},"uniqueItems":true,"minItems":1},"dimensions":{"description":"Product dimensions","type":"object","properties":{"length":{"type":"number"},"width":{"type":"number"},"height":{"type":"number"}},"required":["length","width","height"]},"reviews":{"description":"Reviews for the product","type":"array","items":{"description":"A product review","type":"object","properties":{"rating":{"type":"integer"},"comment":{"type":"string"}},"required":["rating"]}}},"required":["productId","productName","price","dimensions"]}</t>
   </si>
   <si>
@@ -1111,6 +1108,9 @@
   <si>
     <t>To convert a selected cell to a DateTime type, create a DateTimeDetector in memory and specify it when generating a JSON management object.</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{"definitions":{"DIConfiguration":{"type":["object","null"],"properties":{"singletons":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}},"transients":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}}}},"DIItem":{"type":["object","null"],"properties":{"implement_type":{"type":["string","null"]},"service_type":{"type":["string","null"]}}},"ExcelValueConversionConfiguration":{"type":["object","null"],"properties":{"excel_error_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_missing_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_empty_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_string_empty_to":{"type":"string","enum":["excel_error","null","string_empty"]},"null_to":{"type":"string","enum":["excel_empty","string_empty"]},"string_empty_to":{"type":"string","enum":["excel_empty","string_empty"]}}}},"type":"object","properties":{"excel_value_conversion":{"$ref":"#/definitions/ExcelValueConversionConfiguration"},"di_configuration":{"$ref":"#/definitions/DIConfiguration"}}}</t>
   </si>
 </sst>
 </file>
@@ -1675,195 +1675,193 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>4e62a55b-ab11-4eff-9b3a-fd215417b898</stp>
+        <stp>7857bdae-af3d-485c-befc-2f9da794d280</stp>
+        <tr r="E7" s="6"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>6083b218-a3c6-4dbb-86c9-7cc8c9d74bd3</stp>
         <tr r="E9" s="17"/>
       </tp>
+    </main>
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>55598d40-2e6e-41e5-8791-3794a5dcda2f</stp>
-        <tr r="E10" s="15"/>
-        <tr r="E18" s="17"/>
-        <tr r="E9" s="13"/>
+        <stp>8edcb9e1-1134-44ab-9e76-d8d11d3713e7</stp>
+        <tr r="E7" s="7"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>ac57ec78-be9b-46e1-a7cb-ca2faec6f8cc</stp>
+        <stp>7a69f00f-66d3-4ad0-9fac-0e71a240d61d</stp>
+        <tr r="H13" s="5"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>20680dbb-72b9-44f0-97ee-175a1ee764cc</stp>
+        <tr r="E9" s="13"/>
+        <tr r="E18" s="17"/>
+        <tr r="E10" s="15"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>55caab05-c292-4629-a907-e9e33e4981ca</stp>
+        <tr r="E15" s="11"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>1f59f08c-8d1a-405f-848f-ff80d3b176df</stp>
+        <tr r="E38" s="8"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>2338aeb8-dcd6-449e-b6c8-1c59bbf0d8a4</stp>
+        <tr r="E7" s="8"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>a429b3e6-aad7-49e9-8d61-e50eeb625341</stp>
+        <tr r="E10" s="6"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>2c7d448f-892a-4017-ba77-db727288638d</stp>
         <tr r="E7" s="9"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>7863be2f-d043-4387-ab27-d22c600ec2ec</stp>
-        <tr r="E38" s="8"/>
+        <stp>c8ffde60-ff9c-46b9-8318-16e790771945</stp>
+        <tr r="H12" s="5"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>f16b6ba8-ae4b-4a08-8042-00e90d0a6c58</stp>
+        <tr r="E9" s="10"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>62e8627d-67e4-4ebf-a2a3-6874fcd94a86</stp>
-        <tr r="H12" s="5"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>6976d223-c21d-4c10-82ed-400737ee714b</stp>
-        <tr r="E11" s="7"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>019489c0-9e03-42f9-bc71-f686a77d67d8</stp>
+        <stp>6e9c1ae3-14b1-41b6-b9d8-687d5a2a16d4</stp>
         <tr r="E9" s="15"/>
       </tp>
     </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>6887e434-8ab5-40e7-825a-a621e1a4274a</stp>
+        <stp>cd46649d-688c-4012-be71-183d04d42d85</stp>
+        <tr r="H7" s="3"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>0a021a30-9d8a-4399-a69f-1b2155931d78</stp>
+        <tr r="E11" s="8"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>96f5fbcb-05b7-4580-b69e-c7434f6db944</stp>
+        <tr r="E9" s="4"/>
+      </tp>
+      <tp>
+        <v>19</v>
+        <stp/>
+        <stp>c62fc711-63a5-42fa-8c09-002010863b3b</stp>
+        <tr r="D10" s="12"/>
+        <tr r="E7" s="12"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>83763c8a-f65e-4343-b426-cfdcf0599f4b</stp>
+        <tr r="E9" s="2"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>4c67941f-2a3d-4f83-a064-b3a7ae4691ef</stp>
+        <tr r="E9" s="9"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>21250005-2552-4363-8bdc-f4588e221305</stp>
+        <tr r="E15" s="18"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>9089a7ad-caba-41ef-a8af-651466ae0acd</stp>
+        <tr r="E11" s="7"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>7da4bcc6-0363-44b0-82f0-4cf9aa3f3b19</stp>
+        <tr r="E9" s="14"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>7428674e-2f0a-4b7a-b5a4-fe34a2d21f0c</stp>
+        <tr r="H16" s="5"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>c903ffe3-9387-488a-a34d-1617b0be15de</stp>
         <tr r="E15" s="19"/>
       </tp>
+    </main>
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>124b3f52-b669-4bd0-af2d-96568ac0bf88</stp>
-        <tr r="H13" s="5"/>
+        <stp>d6427b55-6676-4ada-8c50-7f6a61ccdb52</stp>
+        <tr r="E18" s="8"/>
       </tp>
     </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
+    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>f67266a3-4407-4093-b6d6-433a4add154e</stp>
-        <tr r="E9" s="10"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>359f128f-ada6-4080-811f-a2fae444ec48</stp>
-        <tr r="E10" s="6"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>52b18cf4-8421-4667-8f96-fb0869299b67</stp>
-        <tr r="E7" s="7"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>95b815e9-455c-48d8-92ee-1312523d64e2</stp>
-        <tr r="E13" s="19"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>6dc4eb0d-6160-4158-8cce-b29c9a131c29</stp>
+        <stp>4eb893d7-0037-4f20-90fb-f4f27b78fd3a</stp>
         <tr r="E12" s="9"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>83ed509d-3cb8-4c59-9a2f-cbb6d153a274</stp>
-        <tr r="E9" s="2"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>9934cbde-15d1-44e2-9087-b8885dbd2fd6</stp>
-        <tr r="E18" s="8"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>328c2339-e633-40d8-a83b-cac04e7d5265</stp>
-        <tr r="E7" s="6"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>44ecde02-30f1-4201-93ba-bf71196d1626</stp>
-        <tr r="H7" s="3"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>53a086b3-eb1a-4b18-8db4-3d5d4dc15b1f</stp>
-        <tr r="E9" s="14"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>3162e316-454d-46a8-960e-ddce71bd235a</stp>
-        <tr r="E11" s="8"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>19d19fa7-4797-4a34-9a6e-3992ea033ff1</stp>
-        <tr r="H16" s="5"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>b23e902f-eb5d-4960-91dc-ab34a1d217ba</stp>
-        <tr r="E9" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>75421c47-d0fd-42c7-8a56-bc8c0621d0f6</stp>
-        <tr r="E15" s="18"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>7018f3c4-67d9-4157-952d-3e837017d634</stp>
-        <tr r="E7" s="8"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_e64d6040cea447b4bfffa3d646f5c498">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>190f99e6-d421-42c3-901f-961654c365a5</stp>
-        <tr r="E15" s="11"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>2d225727-f708-4b26-8c00-748555812c0b</stp>
-        <tr r="E9" s="9"/>
-      </tp>
-      <tp>
-        <v>13</v>
-        <stp/>
-        <stp>37a9d6b1-e0d6-44cd-9993-5b49b340b862</stp>
-        <tr r="D10" s="12"/>
-        <tr r="E7" s="12"/>
+        <stp>0a4c36b5-4b39-4c96-ab24-3bec540ca3a6</stp>
+        <tr r="E13" s="19"/>
       </tp>
     </main>
   </volType>
@@ -2181,7 +2179,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)</f>
@@ -2190,7 +2188,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" s="5" t="str">
         <f ca="1">IF(COUNTIF(D7:D34,"OK")=COUNTA(B7:B34),"OK","NG")</f>
@@ -2199,10 +2197,10 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>62</v>
@@ -2249,7 +2247,7 @@
     </row>
     <row r="10" spans="2:4" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C10" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">INDIRECT("'"&amp;B10&amp;"'!C3")</f>
@@ -2314,7 +2312,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C15" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">INDIRECT("'"&amp;B15&amp;"'!C3")</f>
@@ -2327,7 +2325,7 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C16" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">INDIRECT("'"&amp;B16&amp;"'!C3")</f>
@@ -2340,7 +2338,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">INDIRECT("'"&amp;B17&amp;"'!C3")</f>
@@ -2353,7 +2351,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">INDIRECT("'"&amp;B18&amp;"'!C3")</f>
@@ -2366,7 +2364,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C19" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">INDIRECT("'"&amp;B19&amp;"'!C3")</f>
@@ -2379,7 +2377,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">INDIRECT("'"&amp;B20&amp;"'!C3")</f>
@@ -2392,7 +2390,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C21" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">INDIRECT("'"&amp;B21&amp;"'!C3")</f>
@@ -2405,7 +2403,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C22" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">INDIRECT("'"&amp;B22&amp;"'!C3")</f>
@@ -2467,7 +2465,7 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -2476,10 +2474,10 @@
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -2494,7 +2492,7 @@
     <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>72</v>
@@ -2721,19 +2719,19 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xll.Exlibris.JSON.JSONArray(E6:N12)</f>
-        <v>Newtonsoft.Json.Linq.JArray:5576AE16-2FAB-412B-9235-546108BD7A67</v>
+        <v>Newtonsoft.Json.Linq.JArray:D5B28831-E468-44BB-AEAE-556282F8ADA0</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.55000000000000004">
@@ -2750,7 +2748,7 @@
         <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2786,7 +2784,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -2795,10 +2793,10 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -2813,27 +2811,27 @@
     <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xll.Exlibris.JSON.Schema(E6)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:E26ED978-15D9-41F5-A941-2FFC253288D2</v>
+        <v>Newtonsoft.Json.Schema.JSchema:CEBE4F72-7398-475C-BDEE-28E023C6A358</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -2850,7 +2848,7 @@
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2886,7 +2884,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -2895,10 +2893,10 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -2913,7 +2911,7 @@
     <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema.json"</f>
@@ -2922,19 +2920,19 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.Schema(E6)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:D8D005C4-56FB-43F9-90DC-215926BECB55</v>
+        <v>Newtonsoft.Json.Schema.JSchema:7D6CF8C1-07C9-46D9-B3A7-6D8B9581BBE8</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -2951,7 +2949,7 @@
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2987,7 +2985,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -2996,10 +2994,10 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -3014,7 +3012,7 @@
     <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" t="s">
         <v>129</v>
@@ -3022,19 +3020,19 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xll.Exlibris.JSON.Schema(E6)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:226327D3-9985-47C9-8DDC-6A609A588D76</v>
+        <v>Newtonsoft.Json.Schema.JSchema:354CBB03-03BF-4E05-A4BC-7789BCB9350F</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -3043,7 +3041,7 @@
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xll.Exlibris.JSON.Stringfy(E9)</f>
-        <v>{"definitions":{"ExcelValueConversionConfiguration":{"type":["object","null"],"properties":{"excel_error_to":{"type":"integer","enum":["excel_error","null","string_empty"]},"excel_missing_to":{"type":"integer","enum":["excel_error","null","string_empty"]},"excel_empty_to":{"type":"integer","enum":["excel_error","null","string_empty"]},"excel_string_empty_to":{"type":"integer","enum":["excel_error","null","string_empty"]},"null_to":{"type":"integer","enum":["excel_empty","string_empty"]},"string_empty_to":{"type":"integer","enum":["excel_empty","string_empty"]}}}},"type":"object","properties":{"excel_value_conversion":{"$ref":"#/definitions/ExcelValueConversionConfiguration"}}}</v>
+        <v>{"definitions":{"DIConfiguration":{"type":["object","null"],"properties":{"singletons":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}},"transients":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}}}},"DIItem":{"type":["object","null"],"properties":{"implement_type":{"type":["string","null"]},"service_type":{"type":["string","null"]}}},"ExcelValueConversionConfiguration":{"type":["object","null"],"properties":{"excel_error_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_missing_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_empty_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_string_empty_to":{"type":"string","enum":["excel_error","null","string_empty"]},"null_to":{"type":"string","enum":["excel_empty","string_empty"]},"string_empty_to":{"type":"string","enum":["excel_empty","string_empty"]}}}},"type":"object","properties":{"excel_value_conversion":{"$ref":"#/definitions/ExcelValueConversionConfiguration"},"di_configuration":{"$ref":"#/definitions/DIConfiguration"}}}</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -3051,7 +3049,7 @@
         <v>64</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>143</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3087,7 +3085,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -3096,10 +3094,10 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -3114,7 +3112,7 @@
     <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"product.json"</f>
@@ -3123,7 +3121,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E7" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema.json"</f>
@@ -3132,33 +3130,33 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:FD8F348A-6E1A-439A-B5FF-3C6ECC466038</v>
+        <v>Newtonsoft.Json.Linq.JObject:F7F7470D-DB8A-4248-979B-3F137C47D060</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">_xll.Exlibris.JSON.Schema(E7)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:D8D005C4-56FB-43F9-90DC-215926BECB55</v>
+        <v>Newtonsoft.Json.Schema.JSchema:7D6CF8C1-07C9-46D9-B3A7-6D8B9581BBE8</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E13" t="b" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">_xll.Exlibris.JSON.Validate(E9,E10)</f>
@@ -3200,7 +3198,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -3209,10 +3207,10 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
@@ -3227,7 +3225,7 @@
     <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>130</v>
@@ -3278,7 +3276,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E12" t="s">
         <v>129</v>
@@ -3286,19 +3284,19 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xll.Exlibris.JSON.JSONObject(E6:F11,E12)</f>
-        <v>Newtonsoft.Json.Linq.JObject:5B7CAB41-B82C-4FF5-9BB1-4D2465B7471D</v>
+        <v>Newtonsoft.Json.Linq.JObject:87464541-ADFD-472B-AD0A-47D455C8592A</v>
       </c>
     </row>
   </sheetData>
@@ -3338,7 +3336,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -3347,10 +3345,10 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -3364,13 +3362,13 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="9"/>
       <c r="D7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E7" t="str">
         <f ca="1">FILE_DIR&amp;"product.json"</f>
@@ -3379,16 +3377,16 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.JSONObject(E7)</f>
-        <v>Newtonsoft.Json.Linq.JObject:1E6F9598-4A92-46E2-AC41-3F3DC86EFF64</v>
+        <v>Newtonsoft.Json.Linq.JObject:2088E218-14FF-4A94-92E9-B0774E3868F3</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E10" t="str">
         <f ca="1">FILE_DIR&amp;"product-actual.json"</f>
@@ -3397,15 +3395,15 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E13" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">_xll.Exlibris.JSON.SaveFile(E9,E10)</f>
@@ -3414,12 +3412,12 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E16" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema.json"</f>
@@ -3428,16 +3426,16 @@
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D18" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E18" t="str" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">_xll.Exlibris.JSON.Schema(E16)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:D8D005C4-56FB-43F9-90DC-215926BECB55</v>
+        <v>Newtonsoft.Json.Schema.JSchema:7D6CF8C1-07C9-46D9-B3A7-6D8B9581BBE8</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D19" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E19" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema-actual.json"</f>
@@ -3446,15 +3444,15 @@
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D21" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D22" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E22" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="E22" ca="1">_xll.Exlibris.JSON.SaveFile(E18,E19)</f>
@@ -3463,7 +3461,7 @@
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D24" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E24" t="str">
         <f ca="1">FILE_DIR&amp;"product-expected.json"</f>
@@ -3472,7 +3470,7 @@
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E25" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema-expected.json"</f>
@@ -3495,7 +3493,7 @@
         <v>64</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>63</v>
@@ -3504,7 +3502,7 @@
         <v>64</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="4:10" ht="409.5" x14ac:dyDescent="0.55000000000000004">
@@ -3768,7 +3766,7 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -3777,10 +3775,10 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -3794,30 +3792,30 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" t="s">
         <v>222</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>223</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>224</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>225</v>
-      </c>
-      <c r="H6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E7" s="21">
         <v>44562</v>
       </c>
       <c r="F7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G7" s="22">
         <v>1000</v>
@@ -3828,13 +3826,13 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E8" s="21">
         <v>44563</v>
       </c>
       <c r="F8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G8" s="22">
         <v>500</v>
@@ -3845,13 +3843,13 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E9" s="21">
         <v>44564</v>
       </c>
       <c r="F9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G9" s="22">
         <v>200</v>
@@ -3862,13 +3860,13 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E10" s="21">
         <v>44565</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G10" s="22">
         <v>1500</v>
@@ -3879,19 +3877,19 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E13" t="str" cm="1">
         <f t="array" ref="E13">_xll.Exlibris.Utility.ToDateTime(E7:E10)</f>
-        <v>Exlibris.Excel.DateTimeDetector:EF8117DD-15FA-492F-8B05-DBAC4F9B7B5A</v>
+        <v>Exlibris.Excel.DateTimeDetector:E674F99A-5A78-4865-8FF5-B53DF018E470</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -3900,7 +3898,7 @@
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xll.Exlibris.JSON.JSONArray(D6:H10,E13)</f>
-        <v>Newtonsoft.Json.Linq.JArray:3D360976-2555-42BC-B30B-4B4D67A300F0</v>
+        <v>Newtonsoft.Json.Linq.JArray:E22FF4C2-0616-4926-AE85-3939458B675A</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -3917,7 +3915,7 @@
         <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3955,7 +3953,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -3964,10 +3962,10 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4014,31 +4012,31 @@
     <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" t="str" cm="1">
         <f t="array" ref="D10:E33">_xll.Exlibris.Utility.Objects.Handles(_xll.Exlibris.Utility.TimeAtInterval())</f>
-        <v>Newtonsoft.Json.Linq.JObject:7F991202-195E-4665-9E07-496C20FC58CC</v>
+        <v>Newtonsoft.Json.Linq.JArray:D5B28831-E468-44BB-AEAE-556282F8ADA0</v>
       </c>
       <c r="E10" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.2 create json - path value!H7:H7</v>
+        <v>[1.json-sample-and-test.xlsx]1.9 build json array from table!E15:E15</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D11" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:68B08A40-ABB0-4C90-95D6-AA0E038A9DE5</v>
+        <v>Newtonsoft.Json.Schema.JSchema:7D6CF8C1-07C9-46D9-B3A7-6D8B9581BBE8</v>
       </c>
       <c r="E11" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H12:H12</v>
+        <v>[1.json-sample-and-test.xlsx]1.13 schema - validate!E10:E10</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:4B35F150-7998-4A9E-AA50-33AE48E421DF</v>
+        <v>Newtonsoft.Json.Linq.JObject:BF538929-CFC5-46D8-86C0-CD166B108899</v>
       </c>
       <c r="E12" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E7:E7</v>
+        <v>[1.json-sample-and-test.xlsx]1.5 values - get all values!E7:E7</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:5B7CAB41-B82C-4FF5-9BB1-4D2465B7471D</v>
+        <v>Newtonsoft.Json.Linq.JObject:87464541-ADFD-472B-AD0A-47D455C8592A</v>
       </c>
       <c r="E13" t="str">
         <v>[1.json-sample-and-test.xlsx]1.14 C# object!E15:E15</v>
@@ -4046,7 +4044,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:1E6F9598-4A92-46E2-AC41-3F3DC86EFF64</v>
+        <v>Newtonsoft.Json.Linq.JObject:2088E218-14FF-4A94-92E9-B0774E3868F3</v>
       </c>
       <c r="E14" t="str">
         <v>[1.json-sample-and-test.xlsx]1.15 save file!E9:E9</v>
@@ -4054,95 +4052,95 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:2B1684F9-5A9B-464A-82B8-7624F33EFA6F</v>
+        <v>Newtonsoft.Json.Linq.JObject:F7F7470D-DB8A-4248-979B-3F137C47D060</v>
       </c>
       <c r="E15" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E11:E11</v>
+        <v>[1.json-sample-and-test.xlsx]1.13 schema - validate!E9:E9</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D16" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:DA0E016B-BEE7-4B60-850A-855B0FD317B3</v>
+        <v>Newtonsoft.Json.Linq.JObject:44AB8F38-C073-46ED-8248-AD4D8DBE41C4</v>
       </c>
       <c r="E16" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E7:E7</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D17" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:FD8F348A-6E1A-439A-B5FF-3C6ECC466038</v>
+        <v>Newtonsoft.Json.Linq.JArray:DABC3659-E9B8-4E78-9383-A8C59FF89DE5</v>
       </c>
       <c r="E17" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.13 schema - validate!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D18" t="str">
-        <v>Newtonsoft.Json.Schema.JSchema:226327D3-9985-47C9-8DDC-6A609A588D76</v>
+        <v>Newtonsoft.Json.Linq.JObject:620C362C-5AF8-448E-B015-1C12068C8F4A</v>
       </c>
       <c r="E18" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.12 schema - C# class!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H12:H12</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D19" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:FE48780F-86C9-4C4F-8C4E-7090B23D3CFE</v>
+        <v>Newtonsoft.Json.Linq.JObject:9E39D957-BCB7-4E2F-8248-3EDB4C16A6A3</v>
       </c>
       <c r="E19" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.5 values - get all values!E7:E7</v>
+        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H13:H13</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D20" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:F1A92E20-10DD-4982-A4D0-4257EFF2C5A0</v>
+        <v>Newtonsoft.Json.Linq.JArray:E22FF4C2-0616-4926-AE85-3939458B675A</v>
       </c>
       <c r="E20" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E11:E11</v>
+        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E15:E15</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D21" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:7D99406A-102B-4384-8FB2-0752471B9723</v>
+        <v>Newtonsoft.Json.Linq.JObject:CCB9E626-D183-412D-8093-A4AC23BA6D24</v>
       </c>
       <c r="E21" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H16:H16</v>
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E7:E7</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D22" t="str">
-        <v>Newtonsoft.Json.Schema.JSchema:E26ED978-15D9-41F5-A941-2FFC253288D2</v>
+        <v>Newtonsoft.Json.Linq.JObject:8DC7C7AD-3D8F-4506-97AF-F76B51E797F7</v>
       </c>
       <c r="E22" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.10 schema - json!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.1 create json - json string!E9:E9</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D23" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:1C98B203-98CA-4895-A830-C51003D114F9</v>
+        <v>Newtonsoft.Json.Linq.JObject:C4883E06-EAFF-460B-8FC6-87EBBEC34EC8</v>
       </c>
       <c r="E23" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
+        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E7:E7</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D24" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:AD987A2F-4736-477C-A240-4EA1E99D5570</v>
+        <v>Newtonsoft.Json.Linq.JObject:B46B4AE2-F2BE-4CAF-A917-163DA375CEC3</v>
       </c>
       <c r="E24" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
+        <v>[1.json-sample-and-test.xlsx]1.3 create json - file!E9:E9</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:3F08F95A-DAA0-4C47-BEF4-A32876F65B96</v>
+        <v>Newtonsoft.Json.Linq.JObject:AF90D8BE-9C00-4795-9DDB-0C2626D9B1DB</v>
       </c>
       <c r="E25" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H13:H13</v>
+        <v>[1.json-sample-and-test.xlsx]1.2 create json - path value!H7:H7</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D26" t="str">
-        <v>Exlibris.Excel.DateTimeDetector:EF8117DD-15FA-492F-8B05-DBAC4F9B7B5A</v>
+        <v>Exlibris.Excel.DateTimeDetector:E674F99A-5A78-4865-8FF5-B53DF018E470</v>
       </c>
       <c r="E26" t="str">
         <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E13:E13</v>
@@ -4150,58 +4148,58 @@
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D27" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:3D360976-2555-42BC-B30B-4B4D67A300F0</v>
+        <v>Newtonsoft.Json.Linq.JObject:CD6922A7-FCCD-48ED-A0E4-B54D0B412B3F</v>
       </c>
       <c r="E27" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E15:E15</v>
+        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H16:H16</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D28" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:5576AE16-2FAB-412B-9235-546108BD7A67</v>
+        <v>Newtonsoft.Json.Linq.JArray:B8F0C99E-D887-4E10-A8C9-93E25B132A98</v>
       </c>
       <c r="E28" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.9 build json array from table!E15:E15</v>
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E11:E11</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D29" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:3699941C-1C7D-4F35-BD5D-8DCE9F2A0E09</v>
+        <v>Newtonsoft.Json.Linq.JArray:E1DF4413-5F31-494A-99CC-FF4ACE091097</v>
       </c>
       <c r="E29" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.1 create json - json string!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D30" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:301E5391-E9EC-4A9C-8C58-D7C9BEE70181</v>
+        <v>Newtonsoft.Json.Schema.JSchema:CEBE4F72-7398-475C-BDEE-28E023C6A358</v>
       </c>
       <c r="E30" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E7:E7</v>
+        <v>[1.json-sample-and-test.xlsx]1.10 schema - json!E9:E9</v>
       </c>
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D31" t="str">
-        <v>Newtonsoft.Json.Schema.JSchema:D8D005C4-56FB-43F9-90DC-215926BECB55</v>
+        <v>Newtonsoft.Json.Linq.JObject:F04A3BFA-ACA8-4248-AF28-199B1D266394</v>
       </c>
       <c r="E31" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.11 schema - file!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E11:E11</v>
       </c>
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D32" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:AA1E2024-4828-43F7-93A4-3570646B1F8C</v>
+        <v>Newtonsoft.Json.Linq.JArray:3BCD65A8-6676-4B23-9C08-E354765C23E4</v>
       </c>
       <c r="E32" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.3 create json - file!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E9:E9</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D33" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:DBEB5139-19EF-4704-9C3A-5A55E4BF9F5A</v>
+        <v>Newtonsoft.Json.Schema.JSchema:354CBB03-03BF-4E05-A4BC-7789BCB9350F</v>
       </c>
       <c r="E33" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E7:E7</v>
+        <v>[1.json-sample-and-test.xlsx]1.12 schema - C# class!E9:E9</v>
       </c>
     </row>
   </sheetData>
@@ -4241,7 +4239,7 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",B4),FIND("]",CELL("filename",B4))+1,255)</f>
@@ -4251,10 +4249,10 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9"/>
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -4269,7 +4267,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -4277,19 +4275,19 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:3699941C-1C7D-4F35-BD5D-8DCE9F2A0E09</v>
+        <v>Newtonsoft.Json.Linq.JObject:8DC7C7AD-3D8F-4506-97AF-F76B51E797F7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -4339,7 +4337,7 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -4348,10 +4346,10 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -4365,13 +4363,13 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -4382,11 +4380,11 @@
         <v>3</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H7" t="str" cm="1">
         <f t="array" ref="H7">_xll.Exlibris.JSON.JSONObject(D7:E16)</f>
-        <v>Newtonsoft.Json.Linq.JObject:7F991202-195E-4665-9E07-496C20FC58CC</v>
+        <v>Newtonsoft.Json.Linq.JObject:AF90D8BE-9C00-4795-9DDB-0C2626D9B1DB</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -4507,7 +4505,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -4516,10 +4514,10 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -4534,7 +4532,7 @@
     <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"online-store-products.json"</f>
@@ -4543,19 +4541,19 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:AA1E2024-4828-43F7-93A4-3570646B1F8C</v>
+        <v>Newtonsoft.Json.Linq.JObject:B46B4AE2-F2BE-4CAF-A917-163DA375CEC3</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -4611,7 +4609,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -4620,10 +4618,10 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4638,10 +4636,10 @@
     <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4726,10 +4724,10 @@
       </c>
       <c r="H12" s="14" t="str" cm="1">
         <f t="array" ref="H12">_xll.Exlibris.JSON.JSONObject(D7:E17)</f>
-        <v>Newtonsoft.Json.Linq.JObject:68B08A40-ABB0-4C90-95D6-AA0E038A9DE5</v>
+        <v>Newtonsoft.Json.Linq.JObject:620C362C-5AF8-448E-B015-1C12068C8F4A</v>
       </c>
       <c r="I12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4744,10 +4742,10 @@
       </c>
       <c r="H13" s="14" t="str" cm="1">
         <f t="array" ref="H13">_xll.Exlibris.JSON.JSONObject(D20:E30)</f>
-        <v>Newtonsoft.Json.Linq.JObject:3F08F95A-DAA0-4C47-BEF4-A32876F65B96</v>
+        <v>Newtonsoft.Json.Linq.JObject:9E39D957-BCB7-4E2F-8248-3EDB4C16A6A3</v>
       </c>
       <c r="I13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4766,10 +4764,10 @@
         <v>36</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4780,11 +4778,11 @@
         <v>5</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H16" t="str" cm="1">
         <f t="array" ref="H16">_xll.Exlibris.JSON.JSONObject(G7:H13)</f>
-        <v>Newtonsoft.Json.Linq.JObject:7D99406A-102B-4384-8FB2-0752471B9723</v>
+        <v>Newtonsoft.Json.Linq.JObject:CD6922A7-FCCD-48ED-A0E4-B54D0B412B3F</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.55000000000000004">
@@ -4806,7 +4804,7 @@
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D19" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G19" t="s">
         <v>20</v>
@@ -4940,7 +4938,7 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -4949,10 +4947,10 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -4967,7 +4965,7 @@
     <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -4975,30 +4973,30 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:FE48780F-86C9-4C4F-8C4E-7090B23D3CFE</v>
+        <v>Newtonsoft.Json.Linq.JObject:BF538929-CFC5-46D8-86C0-CD166B108899</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>64</v>
       </c>
       <c r="K9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" ref="E10:F19">_xll.Exlibris.JSON.Values(E7)</f>
@@ -5254,7 +5252,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -5263,10 +5261,10 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
@@ -5281,7 +5279,7 @@
     <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -5289,16 +5287,16 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:DBEB5139-19EF-4704-9C3A-5A55E4BF9F5A</v>
+        <v>Newtonsoft.Json.Linq.JObject:C4883E06-EAFF-460B-8FC6-87EBBEC34EC8</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
         <v>69</v>
@@ -5306,24 +5304,24 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D11" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xll.Exlibris.JSON.Values(E7,E8)</f>
-        <v>Newtonsoft.Json.Linq.JObject:2B1684F9-5A9B-464A-82B8-7624F33EFA6F</v>
+        <v>Newtonsoft.Json.Linq.JObject:F04A3BFA-ACA8-4248-AF28-199B1D266394</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F14" t="str" cm="1">
         <f t="array" ref="F14">_xll.Exlibris.JSON.Stringfy(E11)</f>
@@ -5335,7 +5333,7 @@
         <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -5381,7 +5379,7 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -5390,10 +5388,10 @@
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -5408,7 +5406,7 @@
     <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"books.json"</f>
@@ -5417,35 +5415,35 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:301E5391-E9EC-4A9C-8C58-D7C9BEE70181</v>
+        <v>Newtonsoft.Json.Linq.JObject:44AB8F38-C073-46ED-8248-AD4D8DBE41C4</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.Values(E7,"books")</f>
-        <v>Newtonsoft.Json.Linq.JArray:DA0E016B-BEE7-4B60-850A-855B0FD317B3</v>
+        <v>Newtonsoft.Json.Linq.JArray:3BCD65A8-6676-4B23-9C08-E354765C23E4</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D11" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E12" t="str" cm="1">
         <f t="array" aca="1" ref="E12:N18" ca="1">_xll.Exlibris.JSON.Table(E9)</f>
@@ -5971,7 +5969,7 @@
     </row>
     <row r="29" spans="5:14" x14ac:dyDescent="0.55000000000000004">
       <c r="E29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="5:14" x14ac:dyDescent="0.55000000000000004">
@@ -6302,7 +6300,7 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
@@ -6311,10 +6309,10 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -6329,7 +6327,7 @@
     <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"online-store-products.json"</f>
@@ -6338,32 +6336,32 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:4B35F150-7998-4A9E-AA50-33AE48E421DF</v>
+        <v>Newtonsoft.Json.Linq.JObject:CCB9E626-D183-412D-8093-A4AC23BA6D24</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="E11" t="str" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">_xll.Exlibris.JSON.Values(E7,"products")</f>
-        <v>Newtonsoft.Json.Linq.JArray:F1A92E20-10DD-4982-A4D0-4257EFF2C5A0</v>
+        <v>Newtonsoft.Json.Linq.JArray:B8F0C99E-D887-4E10-A8C9-93E25B132A98</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -6371,18 +6369,18 @@
         <v>72</v>
       </c>
       <c r="F13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" t="s">
         <v>145</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>146</v>
-      </c>
-      <c r="H13" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -6392,15 +6390,15 @@
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D17" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D18" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E18" t="str" cm="1">
         <f t="array" aca="1" ref="E18:H19" ca="1">_xll.Exlibris.JSON.Table(E11,E13:H13,,E15)</f>
@@ -6416,7 +6414,7 @@
       </c>
       <c r="H18" t="str">
         <f ca="1"/>
-        <v>Newtonsoft.Json.Linq.JArray:AD987A2F-4736-477C-A240-4EA1E99D5570</v>
+        <v>Newtonsoft.Json.Linq.JArray:DABC3659-E9B8-4E78-9383-A8C59FF89DE5</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.55000000000000004">
@@ -6434,7 +6432,7 @@
       </c>
       <c r="H19" t="str">
         <f ca="1"/>
-        <v>Newtonsoft.Json.Linq.JArray:1C98B203-98CA-4895-A830-C51003D114F9</v>
+        <v>Newtonsoft.Json.Linq.JArray:E1DF4413-5F31-494A-99CC-FF4ACE091097</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.55000000000000004">
@@ -6455,7 +6453,7 @@
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.55000000000000004">
       <c r="E23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F23" t="s">
         <v>40</v>
@@ -6466,7 +6464,7 @@
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.55000000000000004">
       <c r="E25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.55000000000000004">
@@ -6507,33 +6505,33 @@
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D29" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D30" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.55000000000000004">
       <c r="E31" t="str">
         <f ca="1">E11</f>
-        <v>Newtonsoft.Json.Linq.JArray:F1A92E20-10DD-4982-A4D0-4257EFF2C5A0</v>
+        <v>Newtonsoft.Json.Linq.JArray:B8F0C99E-D887-4E10-A8C9-93E25B132A98</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.55000000000000004">
       <c r="D32" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D34" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.55000000000000004">
@@ -6543,15 +6541,15 @@
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D37" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D38" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E38" t="str" cm="1">
         <f t="array" aca="1" ref="E38:E39" ca="1">_xll.Exlibris.JSON.Table(E31,E33:H33,,E35)</f>
@@ -6581,7 +6579,7 @@
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
In .NET Framework, to avoid errors occurring in ConfigurationBuilder
</commit_message>
<xml_diff>
--- a/samples/1.json-sample-and-test.xlsx
+++ b/samples/1.json-sample-and-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\git\exlibris\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mugenfugafuga\git\exlibris\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CC5CA1-F4E1-4215-B834-6F67F0C82B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CF983D-5E51-4CD0-9220-DF1338EC0C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{70191E0D-F6B7-49FF-9AAA-6C22F5510F3E}"/>
+    <workbookView xWindow="-34510" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{70191E0D-F6B7-49FF-9AAA-6C22F5510F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="top" sheetId="1" r:id="rId1"/>
@@ -1110,7 +1110,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{"definitions":{"DIConfiguration":{"type":["object","null"],"properties":{"singletons":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}},"transients":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}}}},"DIItem":{"type":["object","null"],"properties":{"implement_type":{"type":["string","null"]},"service_type":{"type":["string","null"]}}},"ExcelValueConversionConfiguration":{"type":["object","null"],"properties":{"excel_error_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_missing_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_empty_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_string_empty_to":{"type":"string","enum":["excel_error","null","string_empty"]},"null_to":{"type":"string","enum":["excel_empty","string_empty"]},"string_empty_to":{"type":"string","enum":["excel_empty","string_empty"]}}}},"type":"object","properties":{"excel_value_conversion":{"$ref":"#/definitions/ExcelValueConversionConfiguration"},"di_configuration":{"$ref":"#/definitions/DIConfiguration"}}}</t>
+    <t>{"definitions":{"DIConfiguration":{"type":["object","null"],"properties":{"Singletons":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}},"Transients":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}}},"required":["Singletons","Transients"]},"DIItem":{"type":["object","null"],"properties":{"ImplementType":{"type":["string","null"]},"ServiceType":{"type":["string","null"]}},"required":["ImplementType","ServiceType"]},"ExcelValueConversionConfiguration":{"type":["object","null"],"properties":{"ExcelErrorTo":{"type":"string","enum":["ExcelError","Null","StringEmpty"]},"ExcelMissingTo":{"type":"string","enum":["ExcelError","Null","StringEmpty"]},"ExcelEmptyTo":{"type":"string","enum":["ExcelError","Null","StringEmpty"]},"ExcelStringEmptyTo":{"type":"string","enum":["ExcelError","Null","StringEmpty"]},"NullTo":{"type":"string","enum":["ExcelEmpty","StringEmpty"]},"StringEmptyTo":{"type":"string","enum":["ExcelEmpty","StringEmpty"]}},"required":["ExcelErrorTo","ExcelMissingTo","ExcelEmptyTo","ExcelStringEmptyTo","NullTo","StringEmptyTo"]}},"type":"object","properties":{"ExcelValueConversion":{"$ref":"#/definitions/ExcelValueConversionConfiguration"},"DIConfiguration":{"$ref":"#/definitions/DIConfiguration"}},"required":["ExcelValueConversion","DIConfiguration"]}</t>
   </si>
 </sst>
 </file>
@@ -1675,193 +1675,213 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>7857bdae-af3d-485c-befc-2f9da794d280</stp>
-        <tr r="E7" s="6"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>6083b218-a3c6-4dbb-86c9-7cc8c9d74bd3</stp>
+        <stp>76dd49fc-2d22-40ba-8101-69a0e17ce5bc</stp>
         <tr r="E9" s="17"/>
       </tp>
     </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>8edcb9e1-1134-44ab-9e76-d8d11d3713e7</stp>
+        <stp>16ac52b9-335f-45a1-84b1-2269a131861e</stp>
+        <tr r="E11" s="8"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>92aa6fcb-ace7-4a7c-99f5-8a3b70c273b1</stp>
         <tr r="E7" s="7"/>
       </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>7a69f00f-66d3-4ad0-9fac-0e71a240d61d</stp>
-        <tr r="H13" s="5"/>
+        <stp>330ea8d9-f91f-4a51-92de-a0d36c6868c1</stp>
+        <tr r="E7" s="8"/>
       </tp>
     </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>20680dbb-72b9-44f0-97ee-175a1ee764cc</stp>
+        <stp>3cb4238b-3c1c-46ec-ab29-ba1cd1cc7487</stp>
+        <tr r="E10" s="6"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>30fa14e1-833a-4297-91dc-02c46a2dedc5</stp>
+        <tr r="E9" s="14"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>a8e236ac-18c5-4d8c-9b01-2d22a39cbc18</stp>
+        <tr r="E11" s="7"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>dbc37279-072c-496a-b98d-6394aec1a255</stp>
+        <tr r="E12" s="9"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>bdc621f4-0a8f-4469-94f3-bb672012c59e</stp>
+        <tr r="E9" s="10"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>5e05c03d-f04a-4e48-8c45-9d6a6a66ddec</stp>
+        <tr r="E13" s="19"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>cdf1402f-4ddc-4d5c-b15d-f85e3440eddd</stp>
+        <tr r="E18" s="8"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>8</v>
+        <stp/>
+        <stp>0d9969e2-4fdd-4381-b855-e9ab021b19da</stp>
+        <tr r="D10" s="12"/>
+        <tr r="E7" s="12"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>51ad3bac-6ddf-4ba2-bf0c-beee4759d74d</stp>
+        <tr r="E9" s="15"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>b7c3587d-2d6d-4449-8c0e-df760ec8c525</stp>
+        <tr r="E9" s="2"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>dbf4b470-6060-43ef-9276-bce293ea9b1d</stp>
+        <tr r="H7" s="3"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>3ea85e1c-fc26-4ba1-a918-65acf2277e84</stp>
+        <tr r="E15" s="19"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>953f9fca-f2d5-4f28-9cd3-91be4d355917</stp>
+        <tr r="E15" s="11"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>764ba19e-648f-4e94-a25d-8cea1b399730</stp>
+        <tr r="E9" s="9"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>2e67e87a-d53d-49f7-956f-84a5df000c0b</stp>
+        <tr r="E15" s="18"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>626f4b5a-d8b0-42a8-864e-22b7572a8795</stp>
         <tr r="E9" s="13"/>
         <tr r="E18" s="17"/>
         <tr r="E10" s="15"/>
       </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>55caab05-c292-4629-a907-e9e33e4981ca</stp>
-        <tr r="E15" s="11"/>
+        <stp>c04dc050-e8f2-43b5-8e9c-461572ff8fa0</stp>
+        <tr r="H16" s="5"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>70072863-86f7-4229-8ce7-945b1df21071</stp>
+        <tr r="H13" s="5"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>452ea04d-a075-4192-8993-ac285b035cbf</stp>
+        <tr r="H12" s="5"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>1f59f08c-8d1a-405f-848f-ff80d3b176df</stp>
+        <stp>a4195866-70e1-41b1-b631-5d9f2f446619</stp>
+        <tr r="E7" s="9"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>eb7ec962-bd37-477a-b0e6-7225008601f6</stp>
+        <tr r="E9" s="4"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>6f1dbda9-6048-4692-8239-a0c073040858</stp>
         <tr r="E38" s="8"/>
       </tp>
     </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
+    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>2338aeb8-dcd6-449e-b6c8-1c59bbf0d8a4</stp>
-        <tr r="E7" s="8"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>a429b3e6-aad7-49e9-8d61-e50eeb625341</stp>
-        <tr r="E10" s="6"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>2c7d448f-892a-4017-ba77-db727288638d</stp>
-        <tr r="E7" s="9"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>c8ffde60-ff9c-46b9-8318-16e790771945</stp>
-        <tr r="H12" s="5"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>f16b6ba8-ae4b-4a08-8042-00e90d0a6c58</stp>
-        <tr r="E9" s="10"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>6e9c1ae3-14b1-41b6-b9d8-687d5a2a16d4</stp>
-        <tr r="E9" s="15"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>cd46649d-688c-4012-be71-183d04d42d85</stp>
-        <tr r="H7" s="3"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>0a021a30-9d8a-4399-a69f-1b2155931d78</stp>
-        <tr r="E11" s="8"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>96f5fbcb-05b7-4580-b69e-c7434f6db944</stp>
-        <tr r="E9" s="4"/>
-      </tp>
-      <tp>
-        <v>19</v>
-        <stp/>
-        <stp>c62fc711-63a5-42fa-8c09-002010863b3b</stp>
-        <tr r="D10" s="12"/>
-        <tr r="E7" s="12"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>83763c8a-f65e-4343-b426-cfdcf0599f4b</stp>
-        <tr r="E9" s="2"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>4c67941f-2a3d-4f83-a064-b3a7ae4691ef</stp>
-        <tr r="E9" s="9"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>21250005-2552-4363-8bdc-f4588e221305</stp>
-        <tr r="E15" s="18"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>9089a7ad-caba-41ef-a8af-651466ae0acd</stp>
-        <tr r="E11" s="7"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>7da4bcc6-0363-44b0-82f0-4cf9aa3f3b19</stp>
-        <tr r="E9" s="14"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>7428674e-2f0a-4b7a-b5a4-fe34a2d21f0c</stp>
-        <tr r="H16" s="5"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>c903ffe3-9387-488a-a34d-1617b0be15de</stp>
-        <tr r="E15" s="19"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>d6427b55-6676-4ada-8c50-7f6a61ccdb52</stp>
-        <tr r="E18" s="8"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_3a59cf0281c04e0a80ae3c6cb4c6c8c1">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>4eb893d7-0037-4f20-90fb-f4f27b78fd3a</stp>
-        <tr r="E12" s="9"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>0a4c36b5-4b39-4c96-ab24-3bec540ca3a6</stp>
-        <tr r="E13" s="19"/>
+        <stp>3dc7a95b-20cc-4b50-a021-1fcd9ae7dea1</stp>
+        <tr r="E7" s="6"/>
       </tp>
     </main>
   </volType>
@@ -2169,24 +2189,24 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.375" customWidth="1"/>
     <col min="2" max="2" width="27.25" customWidth="1"/>
-    <col min="3" max="3" width="84.83203125" customWidth="1"/>
+    <col min="3" max="3" width="84.875" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B2" s="6" t="s">
         <v>159</v>
       </c>
       <c r="C2" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)</f>
-        <v>D:\data\git\exlibris\samples\</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>157</v>
       </c>
@@ -2195,7 +2215,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B6" s="18" t="s">
         <v>162</v>
       </c>
@@ -2206,7 +2226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>59</v>
       </c>
@@ -2219,7 +2239,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>60</v>
       </c>
@@ -2232,7 +2252,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
@@ -2245,7 +2265,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:4" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>175</v>
       </c>
@@ -2258,7 +2278,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
@@ -2271,7 +2291,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2284,7 +2304,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>127</v>
       </c>
@@ -2297,7 +2317,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>128</v>
       </c>
@@ -2310,7 +2330,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>156</v>
       </c>
@@ -2323,7 +2343,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>150</v>
       </c>
@@ -2336,7 +2356,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
         <v>151</v>
       </c>
@@ -2349,7 +2369,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>152</v>
       </c>
@@ -2362,7 +2382,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>153</v>
       </c>
@@ -2375,7 +2395,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>154</v>
       </c>
@@ -2388,7 +2408,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B21" s="1" t="s">
         <v>155</v>
       </c>
@@ -2401,7 +2421,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:4" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
         <v>231</v>
       </c>
@@ -2414,7 +2434,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B23" s="1" t="s">
         <v>141</v>
       </c>
@@ -2445,25 +2465,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.4140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -2472,7 +2492,7 @@
         <v>1.9 build json array from table</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -2480,7 +2500,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -2489,7 +2509,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
         <v>167</v>
@@ -2525,7 +2545,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E7" s="12">
         <v>1</v>
       </c>
@@ -2557,7 +2577,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E8" s="12">
         <v>2</v>
       </c>
@@ -2589,7 +2609,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E9" s="12">
         <v>3</v>
       </c>
@@ -2621,7 +2641,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E10" s="12">
         <v>4</v>
       </c>
@@ -2653,7 +2673,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E11" s="12">
         <v>5</v>
       </c>
@@ -2685,7 +2705,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E12" s="12">
         <v>6</v>
       </c>
@@ -2717,7 +2737,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.4">
       <c r="D14" s="7" t="s">
         <v>160</v>
       </c>
@@ -2725,16 +2745,16 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.4">
       <c r="D15" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xll.Exlibris.JSON.JSONArray(E6:N12)</f>
-        <v>Newtonsoft.Json.Linq.JArray:D5B28831-E468-44BB-AEAE-556282F8ADA0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JArray:B0E5B26F-5E7F-4066-AC87-133D55B6596D</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D17" t="s">
         <v>63</v>
       </c>
@@ -2743,7 +2763,7 @@
         <v>[{"id":1,"title":"The Catcher in the Rye","author":"J.D. Salinger","publication_date":"1951-07-16","language":"English","publisher":"Little, Brown and Company","pages":277,"isbn_10":"0316769177","isbn_13":"978-0316769174","genre":"Coming-of-age fiction"},{"id":2,"title":"To Kill a Mockingbird","author":"Harper Lee","publication_date":"1960-07-11","language":"English","publisher":"J. B. Lippincott &amp; Co.","pages":336,"isbn_10":"0060935464","isbn_13":"978-0060935467","genre":"Southern Gothic, Bildungsroman"},{"id":3,"title":"1984","author":"George Orwell","publication_date":"1949-06-08","language":"English","publisher":"Secker &amp; Warburg","pages":328,"isbn_10":"9780451524935","isbn_13":"978-0451524935","genre":"Dystopian, Political fiction"},{"id":4,"title":"One Hundred Years of Solitude","author":"Gabriel García Márquez","publication_date":"1967-05-30","language":"Spanish","publisher":"Harper &amp; Row","pages":417,"isbn_10":"0060883286","isbn_13":"978-0060883287","genre":"Magical Realism"},{"id":5,"title":"The Great Gatsby","author":"F. Scott Fitzgerald","publication_date":"1925-04-10","language":"English","publisher":"Charles Scribner's Sons","pages":218,"isbn_10":"0743273567","isbn_13":"978-0743273565","genre":"Modernist literature"},{"id":6,"title":"War and Peace","author":"Leo Tolstoy","publication_date":"1869-01-01","language":"Russian","publisher":"The Russian Messenger","pages":1225,"isbn_10":"9780140444179","isbn_13":"978-0140444179","genre":"Historical fiction"}]</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D18" t="s">
         <v>64</v>
       </c>
@@ -2774,15 +2794,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -2791,7 +2811,7 @@
         <v>1.10 schema - json</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -2799,7 +2819,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -2808,7 +2828,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
         <v>167</v>
@@ -2817,7 +2837,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D8" s="7" t="s">
         <v>160</v>
       </c>
@@ -2825,16 +2845,16 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D9" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xll.Exlibris.JSON.Schema(E6)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:CEBE4F72-7398-475C-BDEE-28E023C6A358</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Schema.JSchema:11924608-6950-4AE9-8914-AC780E185A31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -2843,7 +2863,7 @@
         <v>{"$schema":"http://json-schema.org/draft-07/schema#","$id":"http://example.com/product.schema.json","title":"Product","description":"A product from Acme's catalog","type":"object","additionalProperties":false,"properties":{"productId":{"description":"The unique identifier for a product","type":"integer"},"productName":{"description":"Name of the product","type":"string"},"price":{"description":"The price of the product","type":"number","exclusiveMinimum":0.0},"tags":{"description":"Tags for the product","type":"array","items":{"type":"string"},"uniqueItems":true,"minItems":1},"dimensions":{"description":"Product dimensions","type":"object","properties":{"length":{"type":"number"},"width":{"type":"number"},"height":{"type":"number"}},"required":["length","width","height"]},"reviews":{"description":"Reviews for the product","type":"array","items":{"description":"A product review","type":"object","properties":{"rating":{"type":"integer"},"comment":{"type":"string"}},"required":["rating"]}}},"required":["productId","productName","price","dimensions"]}</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
         <v>20</v>
       </c>
@@ -2874,15 +2894,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -2891,7 +2911,7 @@
         <v>1.11 schema - file</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -2899,7 +2919,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -2908,17 +2928,17 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
         <v>167</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema.json"</f>
-        <v>D:\data\git\exlibris\samples\product-schema.json</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product-schema.json</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D8" s="7" t="s">
         <v>160</v>
       </c>
@@ -2926,16 +2946,16 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D9" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.Schema(E6)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:7D6CF8C1-07C9-46D9-B3A7-6D8B9581BBE8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Schema.JSchema:DFDB3C8C-F985-438F-B459-0738F3271A83</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -2944,7 +2964,7 @@
         <v>{"$schema":"http://json-schema.org/draft-07/schema#","$id":"http://example.com/product.schema.json","title":"Product","description":"A product from Acme's catalog","type":"object","additionalProperties":false,"properties":{"productId":{"description":"The unique identifier for a product","type":"integer"},"productName":{"description":"Name of the product","type":"string"},"price":{"description":"The price of the product","type":"number","exclusiveMinimum":0.0},"tags":{"description":"Tags for the product","type":"array","items":{"type":"string"},"uniqueItems":true,"minItems":1},"dimensions":{"description":"Product dimensions","type":"object","properties":{"length":{"type":"number"},"width":{"type":"number"},"height":{"type":"number"}},"required":["length","width","height"]},"reviews":{"description":"Reviews for the product","type":"array","items":{"description":"A product review","type":"object","properties":{"rating":{"type":"integer"},"comment":{"type":"string"}},"required":["rating"]}}},"required":["productId","productName","price","dimensions"]}</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
         <v>20</v>
       </c>
@@ -2975,15 +2995,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -2992,7 +3012,7 @@
         <v>1.12 schema - C# class</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -3000,7 +3020,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -3009,7 +3029,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
         <v>167</v>
@@ -3018,7 +3038,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D8" s="7" t="s">
         <v>160</v>
       </c>
@@ -3026,25 +3046,25 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D9" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xll.Exlibris.JSON.Schema(E6)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:354CBB03-03BF-4E05-A4BC-7789BCB9350F</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Schema.JSchema:0090EFF0-BE9E-4187-8D72-4B0E8E4C8359</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
         <v>63</v>
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xll.Exlibris.JSON.Stringfy(E9)</f>
-        <v>{"definitions":{"DIConfiguration":{"type":["object","null"],"properties":{"singletons":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}},"transients":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}}}},"DIItem":{"type":["object","null"],"properties":{"implement_type":{"type":["string","null"]},"service_type":{"type":["string","null"]}}},"ExcelValueConversionConfiguration":{"type":["object","null"],"properties":{"excel_error_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_missing_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_empty_to":{"type":"string","enum":["excel_error","null","string_empty"]},"excel_string_empty_to":{"type":"string","enum":["excel_error","null","string_empty"]},"null_to":{"type":"string","enum":["excel_empty","string_empty"]},"string_empty_to":{"type":"string","enum":["excel_empty","string_empty"]}}}},"type":"object","properties":{"excel_value_conversion":{"$ref":"#/definitions/ExcelValueConversionConfiguration"},"di_configuration":{"$ref":"#/definitions/DIConfiguration"}}}</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>{"definitions":{"DIConfiguration":{"type":["object","null"],"properties":{"Singletons":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}},"Transients":{"type":["array","null"],"items":{"$ref":"#/definitions/DIItem"}}},"required":["Singletons","Transients"]},"DIItem":{"type":["object","null"],"properties":{"ImplementType":{"type":["string","null"]},"ServiceType":{"type":["string","null"]}},"required":["ImplementType","ServiceType"]},"ExcelValueConversionConfiguration":{"type":["object","null"],"properties":{"ExcelErrorTo":{"type":"string","enum":["ExcelError","Null","StringEmpty"]},"ExcelMissingTo":{"type":"string","enum":["ExcelError","Null","StringEmpty"]},"ExcelEmptyTo":{"type":"string","enum":["ExcelError","Null","StringEmpty"]},"ExcelStringEmptyTo":{"type":"string","enum":["ExcelError","Null","StringEmpty"]},"NullTo":{"type":"string","enum":["ExcelEmpty","StringEmpty"]},"StringEmptyTo":{"type":"string","enum":["ExcelEmpty","StringEmpty"]}},"required":["ExcelErrorTo","ExcelMissingTo","ExcelEmptyTo","ExcelStringEmptyTo","NullTo","StringEmptyTo"]}},"type":"object","properties":{"ExcelValueConversion":{"$ref":"#/definitions/ExcelValueConversionConfiguration"},"DIConfiguration":{"$ref":"#/definitions/DIConfiguration"}},"required":["ExcelValueConversion","DIConfiguration"]}</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
         <v>64</v>
       </c>
@@ -3075,15 +3095,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="24.58203125" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="24.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -3092,7 +3112,7 @@
         <v>1.13 schema - validate</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -3100,7 +3120,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -3109,44 +3129,44 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
         <v>188</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"product.json"</f>
-        <v>D:\data\git\exlibris\samples\product.json</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product.json</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
         <v>208</v>
       </c>
       <c r="E7" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema.json"</f>
-        <v>D:\data\git\exlibris\samples\product-schema.json</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product-schema.json</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D9" s="7" t="s">
         <v>209</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:F7F7470D-DB8A-4248-979B-3F137C47D060</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:E91FB160-1AB1-4589-A839-86182402D150</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D10" s="7" t="s">
         <v>210</v>
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">_xll.Exlibris.JSON.Schema(E7)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:7D6CF8C1-07C9-46D9-B3A7-6D8B9581BBE8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Schema.JSchema:DFDB3C8C-F985-438F-B459-0738F3271A83</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D12" s="7" t="s">
         <v>160</v>
       </c>
@@ -3154,7 +3174,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D13" s="7" t="s">
         <v>164</v>
       </c>
@@ -3186,17 +3206,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -3205,7 +3225,7 @@
         <v>1.14 C# object</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -3213,7 +3233,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -3222,7 +3242,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
         <v>180</v>
@@ -3234,7 +3254,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E7" s="12" t="s">
         <v>132</v>
       </c>
@@ -3242,7 +3262,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E8" s="12" t="s">
         <v>134</v>
       </c>
@@ -3250,7 +3270,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E9" s="12" t="s">
         <v>135</v>
       </c>
@@ -3258,7 +3278,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E10" s="12" t="s">
         <v>136</v>
       </c>
@@ -3266,7 +3286,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E11" s="12" t="s">
         <v>138</v>
       </c>
@@ -3274,7 +3294,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D12" s="7" t="s">
         <v>181</v>
       </c>
@@ -3282,7 +3302,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D14" s="7" t="s">
         <v>160</v>
       </c>
@@ -3290,13 +3310,13 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D15" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xll.Exlibris.JSON.JSONObject(E6:F11,E12)</f>
-        <v>Newtonsoft.Json.Linq.JObject:87464541-ADFD-472B-AD0A-47D455C8592A</v>
+        <v>Newtonsoft.Json.Linq.JObject:27163A93-72F6-42ED-AB99-5D7B55B233E1</v>
       </c>
     </row>
   </sheetData>
@@ -3322,19 +3342,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.9140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="9" width="34.4140625" customWidth="1"/>
-    <col min="10" max="10" width="11.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="5" width="22.625" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.625" customWidth="1"/>
+    <col min="8" max="9" width="34.375" customWidth="1"/>
+    <col min="10" max="10" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -3343,7 +3363,7 @@
         <v>1.15 save file</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -3351,7 +3371,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -3360,40 +3380,40 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D6" s="16" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C7" s="9"/>
       <c r="D7" t="s">
         <v>188</v>
       </c>
       <c r="E7" t="str">
         <f ca="1">FILE_DIR&amp;"product.json"</f>
-        <v>D:\data\git\exlibris\samples\product.json</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product.json</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D9" s="7" t="s">
         <v>180</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.JSONObject(E7)</f>
-        <v>Newtonsoft.Json.Linq.JObject:2088E218-14FF-4A94-92E9-B0774E3868F3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:85B92C01-5C24-4C6E-AACB-94529408E155</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D10" s="7" t="s">
         <v>181</v>
       </c>
       <c r="E10" t="str">
         <f ca="1">FILE_DIR&amp;"product-actual.json"</f>
-        <v>D:\data\git\exlibris\samples\product-actual.json</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product-actual.json</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D12" s="7" t="s">
         <v>160</v>
       </c>
@@ -3401,48 +3421,48 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D13" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E13" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">_xll.Exlibris.JSON.SaveFile(E9,E10)</f>
-        <v>D:\data\git\exlibris\samples\product-actual.json</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product-actual.json</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D15" s="16" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D16" t="s">
         <v>208</v>
       </c>
       <c r="E16" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema.json"</f>
-        <v>D:\data\git\exlibris\samples\product-schema.json</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product-schema.json</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.4">
       <c r="D18" s="7" t="s">
         <v>180</v>
       </c>
       <c r="E18" t="str" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">_xll.Exlibris.JSON.Schema(E16)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:7D6CF8C1-07C9-46D9-B3A7-6D8B9581BBE8</v>
-      </c>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Schema.JSchema:DFDB3C8C-F985-438F-B459-0738F3271A83</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.4">
       <c r="D19" s="7" t="s">
         <v>181</v>
       </c>
       <c r="E19" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema-actual.json"</f>
-        <v>D:\data\git\exlibris\samples\product-schema-actual.json</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product-schema-actual.json</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.4">
       <c r="D21" s="7" t="s">
         <v>160</v>
       </c>
@@ -3450,34 +3470,34 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="4:10" x14ac:dyDescent="0.4">
       <c r="D22" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E22" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="E22" ca="1">_xll.Exlibris.JSON.SaveFile(E18,E19)</f>
-        <v>D:\data\git\exlibris\samples\product-schema-actual.json</v>
-      </c>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product-schema-actual.json</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.4">
       <c r="D24" s="7" t="s">
         <v>218</v>
       </c>
       <c r="E24" t="str">
         <f ca="1">FILE_DIR&amp;"product-expected.json"</f>
-        <v>D:\data\git\exlibris\samples\product-expected.json</v>
-      </c>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product-expected.json</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.4">
       <c r="D25" s="7" t="s">
         <v>219</v>
       </c>
       <c r="E25" t="str">
         <f ca="1">FILE_DIR&amp;"product-schema-expected.json"</f>
-        <v>D:\data\git\exlibris\samples\product-schema-expected.json</v>
-      </c>
-    </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\product-schema-expected.json</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.4">
       <c r="D27" t="s">
         <v>19</v>
       </c>
@@ -3485,7 +3505,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.4">
       <c r="D28" s="7" t="s">
         <v>63</v>
       </c>
@@ -3505,7 +3525,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="4:10" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="4:10" ht="409.5" x14ac:dyDescent="0.4">
       <c r="D29" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="D29" ca="1">_xll.Exlibris.Utility.LoadText(E13,FALSE)</f>
         <v>{_x000D_
@@ -3752,19 +3772,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -3773,7 +3793,7 @@
         <v>1.16 DateTime</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -3781,7 +3801,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -3790,7 +3810,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D6" t="s">
         <v>221</v>
       </c>
@@ -3807,7 +3827,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
         <v>226</v>
       </c>
@@ -3824,7 +3844,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D8" t="s">
         <v>226</v>
       </c>
@@ -3841,7 +3861,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
         <v>226</v>
       </c>
@@ -3858,7 +3878,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
         <v>226</v>
       </c>
@@ -3875,7 +3895,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D12" s="7" t="s">
         <v>160</v>
       </c>
@@ -3883,25 +3903,25 @@
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D13" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E13" t="str" cm="1">
         <f t="array" ref="E13">_xll.Exlibris.Utility.ToDateTime(E7:E10)</f>
-        <v>Exlibris.Excel.DateTimeDetector:E674F99A-5A78-4865-8FF5-B53DF018E470</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>Exlibris.Excel.DateTimeDetector:0FCBAC64-1181-4EFA-BDBD-7CC94C701100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
         <v>19</v>
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xll.Exlibris.JSON.JSONArray(D6:H10,E13)</f>
-        <v>Newtonsoft.Json.Linq.JArray:E22FF4C2-0616-4926-AE85-3939458B675A</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JArray:F9339A72-3EBF-4A90-AAEA-3223F6521347</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D16" t="s">
         <v>63</v>
       </c>
@@ -3910,7 +3930,7 @@
         <v>[{"Account Number":"123-4567890"," Transaction Date":"2022-01-01T00:00:00"," Transaction Type":" Deposit"," Transaction Amount":1000," Balance":1000},{"Account Number":"123-4567890"," Transaction Date":"2022-01-02T00:00:00"," Transaction Type":" Withdrawal"," Transaction Amount":500," Balance":500},{"Account Number":"123-4567890"," Transaction Date":"2022-01-03T00:00:00"," Transaction Type":" Withdrawal"," Transaction Amount":200," Balance":300},{"Account Number":"123-4567890"," Transaction Date":"2022-01-04T00:00:00"," Transaction Type":" Deposit"," Transaction Amount":1500," Balance":1800}]</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D17" t="s">
         <v>64</v>
       </c>
@@ -3941,17 +3961,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="66.9140625" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="33.375" customWidth="1"/>
+    <col min="5" max="5" width="66.875" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -3960,7 +3980,7 @@
         <v>1.99 misc</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -3968,7 +3988,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -3977,7 +3997,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D6" s="7" t="s">
         <v>63</v>
       </c>
@@ -3988,7 +4008,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
         <v>139</v>
       </c>
@@ -4004,202 +4024,202 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D10" t="str" cm="1">
         <f t="array" ref="D10:E33">_xll.Exlibris.Utility.Objects.Handles(_xll.Exlibris.Utility.TimeAtInterval())</f>
-        <v>Newtonsoft.Json.Linq.JArray:D5B28831-E468-44BB-AEAE-556282F8ADA0</v>
+        <v>Newtonsoft.Json.Schema.JSchema:11924608-6950-4AE9-8914-AC780E185A31</v>
       </c>
       <c r="E10" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.10 schema - json!E9:E9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D11" t="str">
+        <v>Newtonsoft.Json.Linq.JObject:2DDAF029-8885-47D7-BDCE-2EBE9383B777</v>
+      </c>
+      <c r="E11" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H12:H12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D12" t="str">
+        <v>Exlibris.Excel.DateTimeDetector:0FCBAC64-1181-4EFA-BDBD-7CC94C701100</v>
+      </c>
+      <c r="E12" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E13:E13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D13" t="str">
+        <v>Newtonsoft.Json.Linq.JArray:B012B4FC-91D1-4183-86FB-7C62C66FABD4</v>
+      </c>
+      <c r="E13" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E9:E9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D14" t="str">
+        <v>Newtonsoft.Json.Linq.JArray:015DD6B2-405B-4E4D-AE18-F4C4BD368358</v>
+      </c>
+      <c r="E14" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D15" t="str">
+        <v>Newtonsoft.Json.Linq.JObject:85B92C01-5C24-4C6E-AACB-94529408E155</v>
+      </c>
+      <c r="E15" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.15 save file!E9:E9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="D16" t="str">
+        <v>Newtonsoft.Json.Linq.JObject:E91FB160-1AB1-4589-A839-86182402D150</v>
+      </c>
+      <c r="E16" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.13 schema - validate!E9:E9</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D17" t="str">
+        <v>Newtonsoft.Json.Linq.JObject:937D0D48-B66D-42AA-BB34-7674B7E350F8</v>
+      </c>
+      <c r="E17" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E7:E7</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D18" t="str">
+        <v>Newtonsoft.Json.Linq.JArray:B0E5B26F-5E7F-4066-AC87-133D55B6596D</v>
+      </c>
+      <c r="E18" t="str">
         <v>[1.json-sample-and-test.xlsx]1.9 build json array from table!E15:E15</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="D11" t="str">
-        <v>Newtonsoft.Json.Schema.JSchema:7D6CF8C1-07C9-46D9-B3A7-6D8B9581BBE8</v>
-      </c>
-      <c r="E11" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.13 schema - validate!E10:E10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="D12" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:BF538929-CFC5-46D8-86C0-CD166B108899</v>
-      </c>
-      <c r="E12" t="str">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D19" t="str">
+        <v>Newtonsoft.Json.Linq.JArray:0B767DCE-91EC-45C5-BEE4-8D4A786BC76A</v>
+      </c>
+      <c r="E19" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E11:E11</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D20" t="str">
+        <v>Newtonsoft.Json.Linq.JObject:4FB3877A-A507-4DFC-B89D-1729CB373498</v>
+      </c>
+      <c r="E20" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.1 create json - json string!E9:E9</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D21" t="str">
+        <v>Newtonsoft.Json.Linq.JObject:B662A062-AF77-471E-93C0-612185DB2205</v>
+      </c>
+      <c r="E21" t="str">
         <v>[1.json-sample-and-test.xlsx]1.5 values - get all values!E7:E7</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="D13" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:87464541-ADFD-472B-AD0A-47D455C8592A</v>
-      </c>
-      <c r="E13" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.14 C# object!E15:E15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="D14" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:2088E218-14FF-4A94-92E9-B0774E3868F3</v>
-      </c>
-      <c r="E14" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.15 save file!E9:E9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="D15" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:F7F7470D-DB8A-4248-979B-3F137C47D060</v>
-      </c>
-      <c r="E15" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.13 schema - validate!E9:E9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="D16" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:44AB8F38-C073-46ED-8248-AD4D8DBE41C4</v>
-      </c>
-      <c r="E16" t="str">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D22" t="str">
+        <v>Newtonsoft.Json.Linq.JObject:874C8ECB-E43E-4947-9FDC-2797EF123EEA</v>
+      </c>
+      <c r="E22" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.3 create json - file!E9:E9</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D23" t="str">
+        <v>Newtonsoft.Json.Linq.JArray:F9339A72-3EBF-4A90-AAEA-3223F6521347</v>
+      </c>
+      <c r="E23" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E15:E15</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D24" t="str">
+        <v>Newtonsoft.Json.Linq.JObject:1B7C64D2-771F-4AB0-820E-68E94DB179AA</v>
+      </c>
+      <c r="E24" t="str">
         <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E7:E7</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D17" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:DABC3659-E9B8-4E78-9383-A8C59FF89DE5</v>
-      </c>
-      <c r="E17" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D18" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:620C362C-5AF8-448E-B015-1C12068C8F4A</v>
-      </c>
-      <c r="E18" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H12:H12</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D19" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:9E39D957-BCB7-4E2F-8248-3EDB4C16A6A3</v>
-      </c>
-      <c r="E19" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H13:H13</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D20" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:E22FF4C2-0616-4926-AE85-3939458B675A</v>
-      </c>
-      <c r="E20" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E15:E15</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D21" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:CCB9E626-D183-412D-8093-A4AC23BA6D24</v>
-      </c>
-      <c r="E21" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E7:E7</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D22" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:8DC7C7AD-3D8F-4506-97AF-F76B51E797F7</v>
-      </c>
-      <c r="E22" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.1 create json - json string!E9:E9</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D23" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:C4883E06-EAFF-460B-8FC6-87EBBEC34EC8</v>
-      </c>
-      <c r="E23" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E7:E7</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D24" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:B46B4AE2-F2BE-4CAF-A917-163DA375CEC3</v>
-      </c>
-      <c r="E24" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.3 create json - file!E9:E9</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D25" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:AF90D8BE-9C00-4795-9DDB-0C2626D9B1DB</v>
+        <v>Newtonsoft.Json.Linq.JObject:AB1399E6-6E19-43E5-B0CF-53071E03D3CE</v>
       </c>
       <c r="E25" t="str">
         <v>[1.json-sample-and-test.xlsx]1.2 create json - path value!H7:H7</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D26" t="str">
-        <v>Exlibris.Excel.DateTimeDetector:E674F99A-5A78-4865-8FF5-B53DF018E470</v>
+        <v>Newtonsoft.Json.Schema.JSchema:0090EFF0-BE9E-4187-8D72-4B0E8E4C8359</v>
       </c>
       <c r="E26" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E13:E13</v>
-      </c>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+        <v>[1.json-sample-and-test.xlsx]1.12 schema - C# class!E9:E9</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D27" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:CD6922A7-FCCD-48ED-A0E4-B54D0B412B3F</v>
+        <v>Newtonsoft.Json.Linq.JObject:A62061E7-1B30-4CD0-9C62-86ABFBCC5AB0</v>
       </c>
       <c r="E27" t="str">
+        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E11:E11</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D28" t="str">
+        <v>Newtonsoft.Json.Linq.JObject:F8029AC6-25BB-4419-810F-8D17AFC3593C</v>
+      </c>
+      <c r="E28" t="str">
         <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H16:H16</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D28" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:B8F0C99E-D887-4E10-A8C9-93E25B132A98</v>
-      </c>
-      <c r="E28" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E11:E11</v>
-      </c>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D29" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:E1DF4413-5F31-494A-99CC-FF4ACE091097</v>
+        <v>Newtonsoft.Json.Linq.JArray:CAF9E791-A616-4549-BC67-DCB6B001549C</v>
       </c>
       <c r="E29" t="str">
         <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
       </c>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D30" t="str">
-        <v>Newtonsoft.Json.Schema.JSchema:CEBE4F72-7398-475C-BDEE-28E023C6A358</v>
+        <v>Newtonsoft.Json.Linq.JObject:80D52F5D-E26D-495A-A984-1BB0A6F13BDE</v>
       </c>
       <c r="E30" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.10 schema - json!E9:E9</v>
-      </c>
-    </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H13:H13</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D31" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:F04A3BFA-ACA8-4248-AF28-199B1D266394</v>
+        <v>Newtonsoft.Json.Linq.JObject:27163A93-72F6-42ED-AB99-5D7B55B233E1</v>
       </c>
       <c r="E31" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E11:E11</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+        <v>[1.json-sample-and-test.xlsx]1.14 C# object!E15:E15</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D32" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:3BCD65A8-6676-4B23-9C08-E354765C23E4</v>
+        <v>Newtonsoft.Json.Schema.JSchema:DFDB3C8C-F985-438F-B459-0738F3271A83</v>
       </c>
       <c r="E32" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E9:E9</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+        <v>[1.json-sample-and-test.xlsx]1.13 schema - validate!E10:E10</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D33" t="str">
-        <v>Newtonsoft.Json.Schema.JSchema:354CBB03-03BF-4E05-A4BC-7789BCB9350F</v>
+        <v>Newtonsoft.Json.Linq.JObject:E11B8F8D-C6AA-4489-BA8F-2BB90EEF79AC</v>
       </c>
       <c r="E33" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.12 schema - C# class!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E7:E7</v>
       </c>
     </row>
   </sheetData>
@@ -4228,15 +4248,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
         <v>162</v>
@@ -4246,7 +4266,7 @@
         <v>1.1 create json - json string</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="9"/>
       <c r="B3" s="10" t="s">
         <v>163</v>
@@ -4255,7 +4275,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
         <v>1</v>
@@ -4265,7 +4285,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D6" s="7" t="s">
         <v>167</v>
       </c>
@@ -4273,7 +4293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D8" s="7" t="s">
         <v>160</v>
       </c>
@@ -4281,16 +4301,16 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D9" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:8DC7C7AD-3D8F-4506-97AF-F76B51E797F7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:4FB3877A-A507-4DFC-B89D-1729CB373498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -4299,7 +4319,7 @@
         <v>{"name":"John","age":30,"city":"New York","hobbies":["reading","writing","traveling"],"isMarried":true,"spouse":{"name":"Jane","age":28,"city":"Los Angeles"}}</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
         <v>20</v>
       </c>
@@ -4325,17 +4345,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
     <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.4140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -4344,7 +4364,7 @@
         <v>1.2 create json - path value</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -4352,7 +4372,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -4361,7 +4381,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D6" s="7" t="s">
         <v>167</v>
       </c>
@@ -4372,7 +4392,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D7" s="14" t="s">
         <v>2</v>
       </c>
@@ -4384,10 +4404,10 @@
       </c>
       <c r="H7" t="str" cm="1">
         <f t="array" ref="H7">_xll.Exlibris.JSON.JSONObject(D7:E16)</f>
-        <v>Newtonsoft.Json.Linq.JObject:AF90D8BE-9C00-4795-9DDB-0C2626D9B1DB</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:AB1399E6-6E19-43E5-B0CF-53071E03D3CE</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D8" s="14" t="s">
         <v>4</v>
       </c>
@@ -4395,7 +4415,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D9" s="14" t="s">
         <v>5</v>
       </c>
@@ -4410,7 +4430,7 @@
         <v>{"name":"John","age":30,"city":"New York","hobbies":["reading","writing","traveling"],"isMarried":true,"spouse":{"name":"Jane","age":28,"city":"Los Angeles"}}</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D10" s="14" t="s">
         <v>7</v>
       </c>
@@ -4424,7 +4444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D11" s="14" t="s">
         <v>9</v>
       </c>
@@ -4432,7 +4452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
@@ -4440,7 +4460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D13" s="14" t="s">
         <v>13</v>
       </c>
@@ -4448,7 +4468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D14" s="14" t="s">
         <v>14</v>
       </c>
@@ -4456,7 +4476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D15" s="14" t="s">
         <v>16</v>
       </c>
@@ -4464,7 +4484,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D16" s="14" t="s">
         <v>17</v>
       </c>
@@ -4495,15 +4515,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -4512,7 +4532,7 @@
         <v>1.3 create json - file</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -4520,7 +4540,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -4529,17 +4549,17 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" s="7" t="s">
         <v>167</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"online-store-products.json"</f>
-        <v>D:\data\git\exlibris\samples\online-store-products.json</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\online-store-products.json</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D8" s="7" t="s">
         <v>160</v>
       </c>
@@ -4547,16 +4567,16 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D9" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:B46B4AE2-F2BE-4CAF-A917-163DA375CEC3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:874C8ECB-E43E-4947-9FDC-2797EF123EEA</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
         <v>21</v>
       </c>
@@ -4565,7 +4585,7 @@
         <v>{"store_name":"My Online Store","address":{"street":"123 Main Street","city":"Anytown","state":"CA","zip":"12345"},"products":[{"id":"1","name":"Product 1","description":"This is a description of product 1.","price":9.99,"image_url":"https://example.com/product1.jpg","reviews":[{"username":"johndoe","rating":4,"comment":"I really liked this product."},{"username":"janedoe","rating":5,"comment":"This is the best product ever!"}]},{"id":"2","name":"Product 2","description":"This is a description of product 2.","price":19.99,"image_url":"https://example.com/product2.jpg","reviews":[{"username":"bobsmith","rating":3,"comment":"This product was okay."},{"username":"sarahjones","rating":2,"comment":"I was not satisfied with this product."}]}]}</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
         <v>20</v>
       </c>
@@ -4596,18 +4616,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
     <col min="4" max="4" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.4140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="68.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -4616,7 +4636,7 @@
         <v>1.4 create json - value as json</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -4624,7 +4644,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -4633,7 +4653,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" s="15" t="s">
         <v>191</v>
@@ -4642,7 +4662,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D7" s="12" t="s">
         <v>23</v>
       </c>
@@ -4656,7 +4676,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D8" s="12" t="s">
         <v>2</v>
       </c>
@@ -4670,7 +4690,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D9" s="12" t="s">
         <v>25</v>
       </c>
@@ -4684,7 +4704,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D10" s="12" t="s">
         <v>27</v>
       </c>
@@ -4698,7 +4718,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D11" s="12" t="s">
         <v>28</v>
       </c>
@@ -4712,7 +4732,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D12" s="12" t="s">
         <v>30</v>
       </c>
@@ -4724,13 +4744,13 @@
       </c>
       <c r="H12" s="14" t="str" cm="1">
         <f t="array" ref="H12">_xll.Exlibris.JSON.JSONObject(D7:E17)</f>
-        <v>Newtonsoft.Json.Linq.JObject:620C362C-5AF8-448E-B015-1C12068C8F4A</v>
+        <v>Newtonsoft.Json.Linq.JObject:2DDAF029-8885-47D7-BDCE-2EBE9383B777</v>
       </c>
       <c r="I12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D13" s="12" t="s">
         <v>32</v>
       </c>
@@ -4742,13 +4762,13 @@
       </c>
       <c r="H13" s="14" t="str" cm="1">
         <f t="array" ref="H13">_xll.Exlibris.JSON.JSONObject(D20:E30)</f>
-        <v>Newtonsoft.Json.Linq.JObject:9E39D957-BCB7-4E2F-8248-3EDB4C16A6A3</v>
+        <v>Newtonsoft.Json.Linq.JObject:80D52F5D-E26D-495A-A984-1BB0A6F13BDE</v>
       </c>
       <c r="I13" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D14" s="12" t="s">
         <v>33</v>
       </c>
@@ -4756,7 +4776,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D15" s="12" t="s">
         <v>35</v>
       </c>
@@ -4770,7 +4790,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D16" s="12" t="s">
         <v>37</v>
       </c>
@@ -4782,10 +4802,10 @@
       </c>
       <c r="H16" t="str" cm="1">
         <f t="array" ref="H16">_xll.Exlibris.JSON.JSONObject(G7:H13)</f>
-        <v>Newtonsoft.Json.Linq.JObject:CD6922A7-FCCD-48ED-A0E4-B54D0B412B3F</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:F8029AC6-25BB-4419-810F-8D17AFC3593C</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D17" s="12" t="s">
         <v>38</v>
       </c>
@@ -4793,7 +4813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.4">
       <c r="G18" t="s">
         <v>21</v>
       </c>
@@ -4802,7 +4822,7 @@
         <v>{"store_name":"My Online Store","address":{"street":"123 Main Street","city":"Anytown","state":"CA","zip":"12345"},"products":[{"id":"1","name":"Product 1","description":"This is a description of product 1.","price":9.99,"image_url":"https://example.com/product1.jpg","reviews":[{"username":"johndoe","rating":4,"comment":"I really liked this product."},{"username":"janedoe","rating":5,"comment":"This is the best product ever!"}]},{"id":"2","name":"Product 2","description":"This is a description of product 2.","price":19.99,"image_url":"https://example.com/product2.jpg","reviews":[{"username":"bobsmith","rating":3,"comment":"This product was okay."},{"username":"sarahjones","rating":2,"comment":"I was not satisfied with this product."}]}]}</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D19" s="15" t="s">
         <v>192</v>
       </c>
@@ -4813,7 +4833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D20" s="12" t="s">
         <v>23</v>
       </c>
@@ -4821,7 +4841,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D21" s="12" t="s">
         <v>2</v>
       </c>
@@ -4829,7 +4849,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D22" s="12" t="s">
         <v>25</v>
       </c>
@@ -4837,7 +4857,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D23" s="12" t="s">
         <v>27</v>
       </c>
@@ -4845,7 +4865,7 @@
         <v>19.989999999999998</v>
       </c>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D24" s="12" t="s">
         <v>28</v>
       </c>
@@ -4853,7 +4873,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D25" s="12" t="s">
         <v>30</v>
       </c>
@@ -4861,7 +4881,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D26" s="12" t="s">
         <v>32</v>
       </c>
@@ -4869,7 +4889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D27" s="12" t="s">
         <v>33</v>
       </c>
@@ -4877,7 +4897,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D28" s="12" t="s">
         <v>35</v>
       </c>
@@ -4885,7 +4905,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D29" s="12" t="s">
         <v>37</v>
       </c>
@@ -4893,7 +4913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D30" s="12" t="s">
         <v>38</v>
       </c>
@@ -4924,19 +4944,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.08203125" customWidth="1"/>
-    <col min="6" max="6" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" customWidth="1"/>
+    <col min="6" max="6" width="11.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -4945,7 +4965,7 @@
         <v>1.5 values - get all values</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -4953,7 +4973,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -4962,7 +4982,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
         <v>176</v>
@@ -4971,16 +4991,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D7" s="7" t="s">
         <v>167</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:BF538929-CFC5-46D8-86C0-CD166B108899</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:B662A062-AF77-471E-93C0-612185DB2205</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D9" s="7" t="s">
         <v>160</v>
       </c>
@@ -4994,7 +5014,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D10" s="7" t="s">
         <v>164</v>
       </c>
@@ -5020,7 +5040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
       <c r="E11" t="str">
         <v>$.age</v>
       </c>
@@ -5042,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
       <c r="E12" t="str">
         <v>$.city</v>
       </c>
@@ -5064,7 +5084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
       <c r="E13" t="str">
         <v>$.hobbies[0]</v>
       </c>
@@ -5086,7 +5106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
       <c r="E14" t="str">
         <v>$.hobbies[1]</v>
       </c>
@@ -5108,7 +5128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
       <c r="E15" t="str">
         <v>$.hobbies[2]</v>
       </c>
@@ -5130,7 +5150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
       <c r="E16" t="str">
         <v>$.isMarried</v>
       </c>
@@ -5152,7 +5172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.4">
       <c r="E17" t="str">
         <v>$.spouse.name</v>
       </c>
@@ -5174,7 +5194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.4">
       <c r="E18" t="str">
         <v>$.spouse.age</v>
       </c>
@@ -5196,7 +5216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.4">
       <c r="E19" t="str">
         <v>$.spouse.city</v>
       </c>
@@ -5241,16 +5261,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="23.125" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -5259,7 +5279,7 @@
         <v>1.6 values - json path</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -5267,7 +5287,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -5276,7 +5296,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
         <v>176</v>
@@ -5285,16 +5305,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D7" s="7" t="s">
         <v>180</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:C4883E06-EAFF-460B-8FC6-87EBBEC34EC8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:E11B8F8D-C6AA-4489-BA8F-2BB90EEF79AC</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D8" s="7" t="s">
         <v>181</v>
       </c>
@@ -5302,7 +5322,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D10" s="7" t="s">
         <v>160</v>
       </c>
@@ -5310,16 +5330,16 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D11" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xll.Exlibris.JSON.Values(E7,E8)</f>
-        <v>Newtonsoft.Json.Linq.JObject:F04A3BFA-ACA8-4248-AF28-199B1D266394</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:A62061E7-1B30-4CD0-9C62-86ABFBCC5AB0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E14" s="7" t="s">
         <v>185</v>
       </c>
@@ -5328,7 +5348,7 @@
         <v>{"id":"1","name":"Product 1","description":"This is a description of product 1.","price":9.99,"image_url":"https://example.com/product1.jpg","reviews":[{"username":"johndoe","rating":4,"comment":"I really liked this product."},{"username":"janedoe","rating":5,"comment":"This is the best product ever!"}]}</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E15" s="7" t="s">
         <v>64</v>
       </c>
@@ -5359,25 +5379,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.58203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="28.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="17.625" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.4140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -5386,7 +5406,7 @@
         <v>1.7 table - json array</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -5394,7 +5414,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -5403,37 +5423,37 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
         <v>188</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"books.json"</f>
-        <v>D:\data\git\exlibris\samples\books.json</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\books.json</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
         <v>188</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:44AB8F38-C073-46ED-8248-AD4D8DBE41C4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:1B7C64D2-771F-4AB0-820E-68E94DB179AA</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.4">
       <c r="D8" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.Values(E7,"books")</f>
-        <v>Newtonsoft.Json.Linq.JArray:3BCD65A8-6676-4B23-9C08-E354765C23E4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JArray:B012B4FC-91D1-4183-86FB-7C62C66FABD4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.4">
       <c r="D11" s="7" t="s">
         <v>160</v>
       </c>
@@ -5441,7 +5461,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.4">
       <c r="D12" s="7" t="s">
         <v>164</v>
       </c>
@@ -5486,7 +5506,7 @@
         <v>genre</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E13">
         <f ca="1"/>
         <v>1</v>
@@ -5528,7 +5548,7 @@
         <v>Coming-of-age fiction</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E14">
         <f ca="1"/>
         <v>2</v>
@@ -5570,7 +5590,7 @@
         <v>Southern Gothic, Bildungsroman</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E15">
         <f ca="1"/>
         <v>3</v>
@@ -5612,7 +5632,7 @@
         <v>Dystopian, Political fiction</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E16">
         <f ca="1"/>
         <v>4</v>
@@ -5654,7 +5674,7 @@
         <v>Magical Realism</v>
       </c>
     </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E17">
         <f ca="1"/>
         <v>5</v>
@@ -5696,7 +5716,7 @@
         <v>Modernist literature</v>
       </c>
     </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E18">
         <f ca="1"/>
         <v>6</v>
@@ -5738,12 +5758,12 @@
         <v>Historical fiction</v>
       </c>
     </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E20" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E21" t="s">
         <v>72</v>
       </c>
@@ -5775,7 +5795,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E22">
         <v>1</v>
       </c>
@@ -5807,7 +5827,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E23">
         <v>2</v>
       </c>
@@ -5839,7 +5859,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E24">
         <v>3</v>
       </c>
@@ -5871,7 +5891,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E25">
         <v>4</v>
       </c>
@@ -5903,7 +5923,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E26">
         <v>5</v>
       </c>
@@ -5935,7 +5955,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E27">
         <v>6</v>
       </c>
@@ -5967,12 +5987,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E29" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E30" t="b">
         <f ca="1">E12=E21</f>
         <v>1</v>
@@ -6014,7 +6034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E31" t="b">
         <f t="shared" ref="E31:N31" ca="1" si="1">E13=E22</f>
         <v>1</v>
@@ -6056,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E32" t="b">
         <f t="shared" ref="E32:N32" ca="1" si="2">E14=E23</f>
         <v>1</v>
@@ -6098,7 +6118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E33" t="b">
         <f t="shared" ref="E33:N33" ca="1" si="3">E15=E24</f>
         <v>1</v>
@@ -6140,7 +6160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E34" t="b">
         <f t="shared" ref="E34:N34" ca="1" si="4">E16=E25</f>
         <v>1</v>
@@ -6182,7 +6202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E35" t="b">
         <f t="shared" ref="E35:N36" ca="1" si="5">E17=E26</f>
         <v>1</v>
@@ -6224,7 +6244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="5:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E36" t="b">
         <f t="shared" ca="1" si="5"/>
         <v>1</v>
@@ -6289,16 +6309,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
     <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="11" width="8.6640625" customWidth="1"/>
+    <col min="5" max="11" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>162</v>
       </c>
@@ -6307,7 +6327,7 @@
         <v>1.8 table - column selection</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>163</v>
       </c>
@@ -6315,7 +6335,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
@@ -6324,47 +6344,47 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
       <c r="D6" t="s">
         <v>188</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">FILE_DIR&amp;"online-store-products.json"</f>
-        <v>D:\data\git\exlibris\samples\online-store-products.json</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>D:\mugenfugafuga\git\exlibris\samples\online-store-products.json</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
         <v>188</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:CCB9E626-D183-412D-8093-A4AC23BA6D24</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JObject:937D0D48-B66D-42AA-BB34-7674B7E350F8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D9" s="16" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D10" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="E11" t="str" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">_xll.Exlibris.JSON.Values(E7,"products")</f>
-        <v>Newtonsoft.Json.Linq.JArray:B8F0C99E-D887-4E10-A8C9-93E25B132A98</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JArray:0B767DCE-91EC-45C5-BEE4-8D4A786BC76A</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D12" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="E13" t="s">
         <v>72</v>
       </c>
@@ -6378,17 +6398,17 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="D14" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="E15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D17" s="7" t="s">
         <v>160</v>
       </c>
@@ -6396,7 +6416,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D18" s="7" t="s">
         <v>164</v>
       </c>
@@ -6414,10 +6434,10 @@
       </c>
       <c r="H18" t="str">
         <f ca="1"/>
-        <v>Newtonsoft.Json.Linq.JArray:DABC3659-E9B8-4E78-9383-A8C59FF89DE5</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JArray:CAF9E791-A616-4549-BC67-DCB6B001549C</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.4">
       <c r="E19" t="str">
         <f ca="1"/>
         <v>2</v>
@@ -6432,15 +6452,15 @@
       </c>
       <c r="H19" t="str">
         <f ca="1"/>
-        <v>Newtonsoft.Json.Linq.JArray:E1DF4413-5F31-494A-99CC-FF4ACE091097</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JArray:015DD6B2-405B-4E4D-AE18-F4C4BD368358</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.4">
       <c r="E21" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.4">
       <c r="E22" t="s">
         <v>70</v>
       </c>
@@ -6451,7 +6471,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.4">
       <c r="E23" t="s">
         <v>148</v>
       </c>
@@ -6462,12 +6482,12 @@
         <v>19.989999999999998</v>
       </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.4">
       <c r="E25" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.4">
       <c r="E26" t="b">
         <f ca="1">E18=E22</f>
         <v>1</v>
@@ -6485,7 +6505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.4">
       <c r="E27" t="b">
         <f t="shared" ref="E27:G27" ca="1" si="1">E19=E23</f>
         <v>1</v>
@@ -6503,43 +6523,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D29" s="16" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D30" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.4">
       <c r="E31" t="str">
         <f ca="1">E11</f>
-        <v>Newtonsoft.Json.Linq.JArray:B8F0C99E-D887-4E10-A8C9-93E25B132A98</v>
-      </c>
-    </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+        <v>Newtonsoft.Json.Linq.JArray:0B767DCE-91EC-45C5-BEE4-8D4A786BC76A</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D32" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.4">
       <c r="E33" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D34" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.4">
       <c r="E35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D37" s="7" t="s">
         <v>160</v>
       </c>
@@ -6547,7 +6567,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D38" s="7" t="s">
         <v>164</v>
       </c>
@@ -6556,39 +6576,39 @@
         <v>Product 1</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.4">
       <c r="E39" t="str">
         <f ca="1"/>
         <v>Product 2</v>
       </c>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.4">
       <c r="E41" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.4">
       <c r="E42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.4">
       <c r="E43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.4">
       <c r="E45" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.4">
       <c r="E46" t="b">
         <f ca="1">E38=E42</f>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="4:5" x14ac:dyDescent="0.4">
       <c r="E47" t="b">
         <f t="shared" ref="E47" ca="1" si="2">E39=E43</f>
         <v>1</v>

</xml_diff>

<commit_message>
do not check ExcelReferences
</commit_message>
<xml_diff>
--- a/samples/1.json-sample-and-test.xlsx
+++ b/samples/1.json-sample-and-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mugenfugafuga\git\exlibris\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CF983D-5E51-4CD0-9220-DF1338EC0C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60AE759-66E3-4DEA-8B23-8342D25EBEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34510" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{70191E0D-F6B7-49FF-9AAA-6C22F5510F3E}"/>
+    <workbookView xWindow="-41388" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{70191E0D-F6B7-49FF-9AAA-6C22F5510F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="top" sheetId="1" r:id="rId1"/>
@@ -1675,213 +1675,178 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>76dd49fc-2d22-40ba-8101-69a0e17ce5bc</stp>
+        <stp>4f2c2940-f33e-4473-928b-c54d71b32439</stp>
+        <tr r="E18" s="8"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>53039c34-c7ba-40ac-9d6c-0e7e9168c7af</stp>
+        <tr r="E7" s="8"/>
+        <tr r="E9" s="4"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>ee7a2156-c3cb-4325-a018-118886e8b151</stp>
+        <tr r="E9" s="13"/>
+        <tr r="E10" s="15"/>
+        <tr r="E18" s="17"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>4dace706-af00-4b07-987b-4b96a5cadaaf</stp>
+        <tr r="E38" s="8"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>83bc1fe5-ed0d-496e-9c49-7ee39f248e46</stp>
+        <tr r="E9" s="15"/>
         <tr r="E9" s="17"/>
       </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>16ac52b9-335f-45a1-84b1-2269a131861e</stp>
-        <tr r="E11" s="8"/>
+        <stp>bd884e27-ff13-4620-a828-023eb3bd9cac</stp>
+        <tr r="E15" s="11"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>92aa6fcb-ace7-4a7c-99f5-8a3b70c273b1</stp>
-        <tr r="E7" s="7"/>
+        <stp>6f5e0ad6-14c6-46ad-8700-d5b9e36c7cf4</stp>
+        <tr r="E9" s="10"/>
       </tp>
     </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>330ea8d9-f91f-4a51-92de-a0d36c6868c1</stp>
-        <tr r="E7" s="8"/>
+        <stp>603983ad-693c-401e-b40e-faec433e69ff</stp>
+        <tr r="E12" s="9"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>6449098b-05dd-43bb-9fe0-6d5a018a4daf</stp>
+        <tr r="E7" s="6"/>
+        <tr r="E9" s="2"/>
       </tp>
     </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>3cb4238b-3c1c-46ec-ab29-ba1cd1cc7487</stp>
-        <tr r="E10" s="6"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>30fa14e1-833a-4297-91dc-02c46a2dedc5</stp>
-        <tr r="E9" s="14"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>a8e236ac-18c5-4d8c-9b01-2d22a39cbc18</stp>
+        <stp>4b591387-b2ab-477e-8383-279a43afbe6c</stp>
         <tr r="E11" s="7"/>
       </tp>
     </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>dbc37279-072c-496a-b98d-6394aec1a255</stp>
-        <tr r="E12" s="9"/>
+        <stp>f4609e97-8f36-49bb-954d-d341c03182a5</stp>
+        <tr r="H12" s="5"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>bdc621f4-0a8f-4469-94f3-bb672012c59e</stp>
-        <tr r="E9" s="10"/>
+        <stp>486a8b26-e596-4306-b496-bf005af4490b</stp>
+        <tr r="H13" s="5"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>90aac6c8-d711-4c6a-9067-bc0c2c29bdb5</stp>
+        <tr r="H16" s="5"/>
       </tp>
     </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>5e05c03d-f04a-4e48-8c45-9d6a6a66ddec</stp>
-        <tr r="E13" s="19"/>
+        <stp>94e12f5e-dabf-4491-b567-ffd5f12db48c</stp>
+        <tr r="E11" s="8"/>
       </tp>
     </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>cdf1402f-4ddc-4d5c-b15d-f85e3440eddd</stp>
-        <tr r="E18" s="8"/>
+        <stp>49719e1e-7489-46e3-9b5b-f770c9525681</stp>
+        <tr r="E9" s="9"/>
       </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
       <tp>
-        <v>8</v>
+        <v>17</v>
         <stp/>
-        <stp>0d9969e2-4fdd-4381-b855-e9ab021b19da</stp>
+        <stp>8937d718-c639-4d3c-b3e7-abb4694b9e3e</stp>
         <tr r="D10" s="12"/>
         <tr r="E7" s="12"/>
       </tp>
     </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>51ad3bac-6ddf-4ba2-bf0c-beee4759d74d</stp>
-        <tr r="E9" s="15"/>
+        <stp>e9939095-e871-4dc4-ab96-5748d33d12d0</stp>
+        <tr r="E7" s="7"/>
       </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>b7c3587d-2d6d-4449-8c0e-df760ec8c525</stp>
-        <tr r="E9" s="2"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>dbf4b470-6060-43ef-9276-bce293ea9b1d</stp>
-        <tr r="H7" s="3"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>3ea85e1c-fc26-4ba1-a918-65acf2277e84</stp>
-        <tr r="E15" s="19"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>953f9fca-f2d5-4f28-9cd3-91be4d355917</stp>
-        <tr r="E15" s="11"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>764ba19e-648f-4e94-a25d-8cea1b399730</stp>
-        <tr r="E9" s="9"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>2e67e87a-d53d-49f7-956f-84a5df000c0b</stp>
+        <stp>e865345e-dfaf-41f8-9b74-4881c1c779dd</stp>
         <tr r="E15" s="18"/>
       </tp>
     </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>626f4b5a-d8b0-42a8-864e-22b7572a8795</stp>
-        <tr r="E9" s="13"/>
-        <tr r="E18" s="17"/>
-        <tr r="E10" s="15"/>
+        <stp>18cbe15e-6acc-4a04-a40f-7b83a5cb1589</stp>
+        <tr r="H7" s="3"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>8ca0fee9-c5e3-4803-a73b-389f142a8175</stp>
+        <tr r="E13" s="19"/>
       </tp>
     </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>c04dc050-e8f2-43b5-8e9c-461572ff8fa0</stp>
-        <tr r="H16" s="5"/>
+        <stp>657f82a8-79f8-4994-b0d5-4bf268450aef</stp>
+        <tr r="E15" s="19"/>
+      </tp>
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>24c936d7-b242-45af-ac99-d3968af6a679</stp>
+        <tr r="E7" s="9"/>
       </tp>
     </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
+    <main first="rtdsrv_6690efc3d90442fab44c00f5a531a8c6">
       <tp>
         <v>1</v>
         <stp/>
-        <stp>70072863-86f7-4229-8ce7-945b1df21071</stp>
-        <tr r="H13" s="5"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>452ea04d-a075-4192-8993-ac285b035cbf</stp>
-        <tr r="H12" s="5"/>
+        <stp>0a99c070-cbb8-44a3-a28d-0e5353ede38a</stp>
+        <tr r="E9" s="14"/>
       </tp>
       <tp>
         <v>1</v>
         <stp/>
-        <stp>a4195866-70e1-41b1-b631-5d9f2f446619</stp>
-        <tr r="E7" s="9"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>eb7ec962-bd37-477a-b0e6-7225008601f6</stp>
-        <tr r="E9" s="4"/>
-      </tp>
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>6f1dbda9-6048-4692-8239-a0c073040858</stp>
-        <tr r="E38" s="8"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_c78724fe63ca455f9f06af5b49b381dd">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>3dc7a95b-20cc-4b50-a021-1fcd9ae7dea1</stp>
-        <tr r="E7" s="6"/>
+        <stp>fd74195d-3268-4ae4-a107-a338321ac469</stp>
+        <tr r="E10" s="6"/>
       </tp>
     </main>
   </volType>
@@ -2751,7 +2716,7 @@
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xll.Exlibris.JSON.JSONArray(E6:N12)</f>
-        <v>Newtonsoft.Json.Linq.JArray:B0E5B26F-5E7F-4066-AC87-133D55B6596D</v>
+        <v>Newtonsoft.Json.Linq.JArray:20A66C27-1B40-402F-BA8B-27E4A623B6F7</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.4">
@@ -2851,7 +2816,7 @@
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xll.Exlibris.JSON.Schema(E6)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:11924608-6950-4AE9-8914-AC780E185A31</v>
+        <v>Newtonsoft.Json.Schema.JSchema:39F20E0D-58C6-4C61-8C16-1D52806DC609</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.4">
@@ -2952,7 +2917,7 @@
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.Schema(E6)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:DFDB3C8C-F985-438F-B459-0738F3271A83</v>
+        <v>Newtonsoft.Json.Schema.JSchema:C3CFF37D-DE59-43D1-8188-524084FC0175</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.4">
@@ -3052,7 +3017,7 @@
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xll.Exlibris.JSON.Schema(E6)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:0090EFF0-BE9E-4187-8D72-4B0E8E4C8359</v>
+        <v>Newtonsoft.Json.Schema.JSchema:53E05FB2-77FE-4201-B49C-12BA5E39F828</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.4">
@@ -3154,7 +3119,7 @@
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:E91FB160-1AB1-4589-A839-86182402D150</v>
+        <v>Newtonsoft.Json.Linq.JObject:FAF0070B-FCBC-400F-B1FF-AEACF4E641A6</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.4">
@@ -3163,7 +3128,7 @@
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">_xll.Exlibris.JSON.Schema(E7)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:DFDB3C8C-F985-438F-B459-0738F3271A83</v>
+        <v>Newtonsoft.Json.Schema.JSchema:C3CFF37D-DE59-43D1-8188-524084FC0175</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.4">
@@ -3316,7 +3281,7 @@
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xll.Exlibris.JSON.JSONObject(E6:F11,E12)</f>
-        <v>Newtonsoft.Json.Linq.JObject:27163A93-72F6-42ED-AB99-5D7B55B233E1</v>
+        <v>Newtonsoft.Json.Linq.JObject:D20596DF-8B28-4743-A22A-17EBB37B42E3</v>
       </c>
     </row>
   </sheetData>
@@ -3401,7 +3366,7 @@
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.JSONObject(E7)</f>
-        <v>Newtonsoft.Json.Linq.JObject:85B92C01-5C24-4C6E-AACB-94529408E155</v>
+        <v>Newtonsoft.Json.Linq.JObject:FAF0070B-FCBC-400F-B1FF-AEACF4E641A6</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.4">
@@ -3450,7 +3415,7 @@
       </c>
       <c r="E18" t="str" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">_xll.Exlibris.JSON.Schema(E16)</f>
-        <v>Newtonsoft.Json.Schema.JSchema:DFDB3C8C-F985-438F-B459-0738F3271A83</v>
+        <v>Newtonsoft.Json.Schema.JSchema:C3CFF37D-DE59-43D1-8188-524084FC0175</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.4">
@@ -3909,7 +3874,7 @@
       </c>
       <c r="E13" t="str" cm="1">
         <f t="array" ref="E13">_xll.Exlibris.Utility.ToDateTime(E7:E10)</f>
-        <v>Exlibris.Excel.DateTimeDetector:0FCBAC64-1181-4EFA-BDBD-7CC94C701100</v>
+        <v>Exlibris.Excel.DateTimeDetector:D4A19CAF-2189-480B-8E0B-6011D299BCD6</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.4">
@@ -3918,7 +3883,7 @@
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xll.Exlibris.JSON.JSONArray(D6:H10,E13)</f>
-        <v>Newtonsoft.Json.Linq.JArray:F9339A72-3EBF-4A90-AAEA-3223F6521347</v>
+        <v>Newtonsoft.Json.Linq.JArray:4495B600-B11C-43DA-8B43-77B71CAC8917</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.4">
@@ -3957,7 +3922,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7028040-FE4D-414D-B44F-31DFB2FA4BFE}">
-  <dimension ref="B2:I33"/>
+  <dimension ref="B2:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4014,10 +3979,10 @@
       </c>
       <c r="E7" cm="1">
         <f t="array" ref="E7">_xll.Exlibris.Utility.Objects.Count(_xll.Exlibris.Utility.TimeAtInterval())</f>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G7">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I7" t="b">
         <f>E7=G7</f>
@@ -4031,195 +3996,171 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D10" t="str" cm="1">
-        <f t="array" ref="D10:E33">_xll.Exlibris.Utility.Objects.Handles(_xll.Exlibris.Utility.TimeAtInterval())</f>
-        <v>Newtonsoft.Json.Schema.JSchema:11924608-6950-4AE9-8914-AC780E185A31</v>
+        <f t="array" ref="D10:E30">_xll.Exlibris.Utility.Objects.Handles(_xll.Exlibris.Utility.TimeAtInterval())</f>
+        <v>Newtonsoft.Json.Linq.JObject:D20596DF-8B28-4743-A22A-17EBB37B42E3</v>
       </c>
       <c r="E10" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.10 schema - json!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.14 C# object!E15:E15</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D11" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:2DDAF029-8885-47D7-BDCE-2EBE9383B777</v>
+        <v>Newtonsoft.Json.Schema.JSchema:53E05FB2-77FE-4201-B49C-12BA5E39F828</v>
       </c>
       <c r="E11" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H12:H12</v>
+        <v>[1.json-sample-and-test.xlsx]1.12 schema - C# class!E9:E9</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D12" t="str">
-        <v>Exlibris.Excel.DateTimeDetector:0FCBAC64-1181-4EFA-BDBD-7CC94C701100</v>
+        <v>Newtonsoft.Json.Linq.JObject:571C32A0-5FB2-45C2-9E91-988580482C9D</v>
       </c>
       <c r="E12" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E13:E13</v>
+        <v>[1.json-sample-and-test.xlsx]1.2 create json - path value!H7:H7</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D13" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:B012B4FC-91D1-4183-86FB-7C62C66FABD4</v>
+        <v>Exlibris.Excel.DateTimeDetector:D4A19CAF-2189-480B-8E0B-6011D299BCD6</v>
       </c>
       <c r="E13" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E13:E13</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D14" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:015DD6B2-405B-4E4D-AE18-F4C4BD368358</v>
+        <v>Newtonsoft.Json.Linq.JObject:FFE0AD41-E9E2-47E3-AED6-512854B26B5D</v>
       </c>
       <c r="E14" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
+        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H16:H16</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D15" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:85B92C01-5C24-4C6E-AACB-94529408E155</v>
+        <v>Newtonsoft.Json.Linq.JObject:A09069D1-7345-496A-A8DE-F25B93803ECB</v>
       </c>
       <c r="E15" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.15 save file!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.1 create json - json string!E9:E9</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D16" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:E91FB160-1AB1-4589-A839-86182402D150</v>
+        <v>Newtonsoft.Json.Linq.JObject:8FFAF5CE-5598-41D8-B92D-8D96793A1335</v>
       </c>
       <c r="E16" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.13 schema - validate!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H13:H13</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D17" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:937D0D48-B66D-42AA-BB34-7674B7E350F8</v>
+        <v>Newtonsoft.Json.Linq.JArray:0127E335-7E9D-41DC-B272-88D82BD2518F</v>
       </c>
       <c r="E17" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E7:E7</v>
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D18" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:B0E5B26F-5E7F-4066-AC87-133D55B6596D</v>
+        <v>Newtonsoft.Json.Schema.JSchema:39F20E0D-58C6-4C61-8C16-1D52806DC609</v>
       </c>
       <c r="E18" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.9 build json array from table!E15:E15</v>
+        <v>[1.json-sample-and-test.xlsx]1.10 schema - json!E9:E9</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D19" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:0B767DCE-91EC-45C5-BEE4-8D4A786BC76A</v>
+        <v>Newtonsoft.Json.Linq.JObject:FAF0070B-FCBC-400F-B1FF-AEACF4E641A6</v>
       </c>
       <c r="E19" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E11:E11</v>
+        <v>[1.json-sample-and-test.xlsx]1.15 save file!E9:E9</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D20" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:4FB3877A-A507-4DFC-B89D-1729CB373498</v>
+        <v>Newtonsoft.Json.Linq.JObject:2AE7519C-62C4-46C7-BD1B-E3C551C19A64</v>
       </c>
       <c r="E20" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.1 create json - json string!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E11:E11</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D21" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:B662A062-AF77-471E-93C0-612185DB2205</v>
+        <v>Newtonsoft.Json.Linq.JArray:89167A74-51DD-46E6-8B70-EE7D5A78C151</v>
       </c>
       <c r="E21" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.5 values - get all values!E7:E7</v>
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E11:E11</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D22" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:874C8ECB-E43E-4947-9FDC-2797EF123EEA</v>
+        <v>Newtonsoft.Json.Linq.JObject:AE75D883-3157-4EEB-8915-9702B1D68161</v>
       </c>
       <c r="E22" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.3 create json - file!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E7:E7</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D23" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:F9339A72-3EBF-4A90-AAEA-3223F6521347</v>
+        <v>Newtonsoft.Json.Linq.JObject:FA9111DF-4793-41EE-AFA5-581C60640511</v>
       </c>
       <c r="E23" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E15:E15</v>
+        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H12:H12</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D24" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:1B7C64D2-771F-4AB0-820E-68E94DB179AA</v>
+        <v>Newtonsoft.Json.Linq.JObject:3E2789DB-452C-4EC2-A1DF-C595278081CC</v>
       </c>
       <c r="E24" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E7:E7</v>
+        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E7:E7</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D25" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:AB1399E6-6E19-43E5-B0CF-53071E03D3CE</v>
+        <v>Newtonsoft.Json.Linq.JArray:20A66C27-1B40-402F-BA8B-27E4A623B6F7</v>
       </c>
       <c r="E25" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.2 create json - path value!H7:H7</v>
+        <v>[1.json-sample-and-test.xlsx]1.9 build json array from table!E15:E15</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D26" t="str">
-        <v>Newtonsoft.Json.Schema.JSchema:0090EFF0-BE9E-4187-8D72-4B0E8E4C8359</v>
+        <v>Newtonsoft.Json.Linq.JArray:4495B600-B11C-43DA-8B43-77B71CAC8917</v>
       </c>
       <c r="E26" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.12 schema - C# class!E9:E9</v>
+        <v>[1.json-sample-and-test.xlsx]1.16 DateTime!E15:E15</v>
       </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D27" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:A62061E7-1B30-4CD0-9C62-86ABFBCC5AB0</v>
+        <v>Newtonsoft.Json.Schema.JSchema:C3CFF37D-DE59-43D1-8188-524084FC0175</v>
       </c>
       <c r="E27" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E11:E11</v>
+        <v>[1.json-sample-and-test.xlsx]1.15 save file!E18:E18</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D28" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:F8029AC6-25BB-4419-810F-8D17AFC3593C</v>
+        <v>Newtonsoft.Json.Linq.JObject:7CA34E63-511D-40BC-888F-440525D8CFEB</v>
       </c>
       <c r="E28" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H16:H16</v>
+        <v>[1.json-sample-and-test.xlsx]1.3 create json - file!E9:E9</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D29" t="str">
-        <v>Newtonsoft.Json.Linq.JArray:CAF9E791-A616-4549-BC67-DCB6B001549C</v>
+        <v>Newtonsoft.Json.Linq.JArray:211C9B86-4B66-496C-A5FB-05869067BB3B</v>
       </c>
       <c r="E29" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
+        <v>[1.json-sample-and-test.xlsx]1.7 table - json array!E9:E9</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D30" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:80D52F5D-E26D-495A-A984-1BB0A6F13BDE</v>
+        <v>Newtonsoft.Json.Linq.JArray:380ACAB5-B8E5-4BA2-A914-43D3ABA895A6</v>
       </c>
       <c r="E30" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.4 create json - value as json!H13:H13</v>
-      </c>
-    </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D31" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:27163A93-72F6-42ED-AB99-5D7B55B233E1</v>
-      </c>
-      <c r="E31" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.14 C# object!E15:E15</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D32" t="str">
-        <v>Newtonsoft.Json.Schema.JSchema:DFDB3C8C-F985-438F-B459-0738F3271A83</v>
-      </c>
-      <c r="E32" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.13 schema - validate!E10:E10</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D33" t="str">
-        <v>Newtonsoft.Json.Linq.JObject:E11B8F8D-C6AA-4489-BA8F-2BB90EEF79AC</v>
-      </c>
-      <c r="E33" t="str">
-        <v>[1.json-sample-and-test.xlsx]1.6 values - json path!E7:E7</v>
+        <v>[1.json-sample-and-test.xlsx]1.8 table - column selection!E18:E18</v>
       </c>
     </row>
   </sheetData>
@@ -4307,7 +4248,7 @@
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:4FB3877A-A507-4DFC-B89D-1729CB373498</v>
+        <v>Newtonsoft.Json.Linq.JObject:A09069D1-7345-496A-A8DE-F25B93803ECB</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
@@ -4404,7 +4345,7 @@
       </c>
       <c r="H7" t="str" cm="1">
         <f t="array" ref="H7">_xll.Exlibris.JSON.JSONObject(D7:E16)</f>
-        <v>Newtonsoft.Json.Linq.JObject:AB1399E6-6E19-43E5-B0CF-53071E03D3CE</v>
+        <v>Newtonsoft.Json.Linq.JObject:571C32A0-5FB2-45C2-9E91-988580482C9D</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
@@ -4573,7 +4514,7 @@
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:874C8ECB-E43E-4947-9FDC-2797EF123EEA</v>
+        <v>Newtonsoft.Json.Linq.JObject:7CA34E63-511D-40BC-888F-440525D8CFEB</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.4">
@@ -4744,7 +4685,7 @@
       </c>
       <c r="H12" s="14" t="str" cm="1">
         <f t="array" ref="H12">_xll.Exlibris.JSON.JSONObject(D7:E17)</f>
-        <v>Newtonsoft.Json.Linq.JObject:2DDAF029-8885-47D7-BDCE-2EBE9383B777</v>
+        <v>Newtonsoft.Json.Linq.JObject:FA9111DF-4793-41EE-AFA5-581C60640511</v>
       </c>
       <c r="I12" t="s">
         <v>173</v>
@@ -4762,7 +4703,7 @@
       </c>
       <c r="H13" s="14" t="str" cm="1">
         <f t="array" ref="H13">_xll.Exlibris.JSON.JSONObject(D20:E30)</f>
-        <v>Newtonsoft.Json.Linq.JObject:80D52F5D-E26D-495A-A984-1BB0A6F13BDE</v>
+        <v>Newtonsoft.Json.Linq.JObject:8FFAF5CE-5598-41D8-B92D-8D96793A1335</v>
       </c>
       <c r="I13" t="s">
         <v>174</v>
@@ -4802,7 +4743,7 @@
       </c>
       <c r="H16" t="str" cm="1">
         <f t="array" ref="H16">_xll.Exlibris.JSON.JSONObject(G7:H13)</f>
-        <v>Newtonsoft.Json.Linq.JObject:F8029AC6-25BB-4419-810F-8D17AFC3593C</v>
+        <v>Newtonsoft.Json.Linq.JObject:FFE0AD41-E9E2-47E3-AED6-512854B26B5D</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.4">
@@ -4997,7 +4938,7 @@
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:B662A062-AF77-471E-93C0-612185DB2205</v>
+        <v>Newtonsoft.Json.Linq.JObject:A09069D1-7345-496A-A8DE-F25B93803ECB</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.4">
@@ -5311,7 +5252,7 @@
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:E11B8F8D-C6AA-4489-BA8F-2BB90EEF79AC</v>
+        <v>Newtonsoft.Json.Linq.JObject:3E2789DB-452C-4EC2-A1DF-C595278081CC</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.4">
@@ -5336,7 +5277,7 @@
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xll.Exlibris.JSON.Values(E7,E8)</f>
-        <v>Newtonsoft.Json.Linq.JObject:A62061E7-1B30-4CD0-9C62-86ABFBCC5AB0</v>
+        <v>Newtonsoft.Json.Linq.JObject:2AE7519C-62C4-46C7-BD1B-E3C551C19A64</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.4">
@@ -5439,7 +5380,7 @@
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:1B7C64D2-771F-4AB0-820E-68E94DB179AA</v>
+        <v>Newtonsoft.Json.Linq.JObject:AE75D883-3157-4EEB-8915-9702B1D68161</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.4">
@@ -5450,7 +5391,7 @@
     <row r="9" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E9" t="str" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">_xll.Exlibris.JSON.Values(E7,"books")</f>
-        <v>Newtonsoft.Json.Linq.JArray:B012B4FC-91D1-4183-86FB-7C62C66FABD4</v>
+        <v>Newtonsoft.Json.Linq.JArray:211C9B86-4B66-496C-A5FB-05869067BB3B</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.4">
@@ -6360,7 +6301,7 @@
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_xll.Exlibris.JSON.JSONObject(E6)</f>
-        <v>Newtonsoft.Json.Linq.JObject:937D0D48-B66D-42AA-BB34-7674B7E350F8</v>
+        <v>Newtonsoft.Json.Linq.JObject:7CA34E63-511D-40BC-888F-440525D8CFEB</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
@@ -6376,7 +6317,7 @@
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="E11" t="str" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">_xll.Exlibris.JSON.Values(E7,"products")</f>
-        <v>Newtonsoft.Json.Linq.JArray:0B767DCE-91EC-45C5-BEE4-8D4A786BC76A</v>
+        <v>Newtonsoft.Json.Linq.JArray:89167A74-51DD-46E6-8B70-EE7D5A78C151</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
@@ -6434,7 +6375,7 @@
       </c>
       <c r="H18" t="str">
         <f ca="1"/>
-        <v>Newtonsoft.Json.Linq.JArray:CAF9E791-A616-4549-BC67-DCB6B001549C</v>
+        <v>Newtonsoft.Json.Linq.JArray:380ACAB5-B8E5-4BA2-A914-43D3ABA895A6</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.4">
@@ -6452,7 +6393,7 @@
       </c>
       <c r="H19" t="str">
         <f ca="1"/>
-        <v>Newtonsoft.Json.Linq.JArray:015DD6B2-405B-4E4D-AE18-F4C4BD368358</v>
+        <v>Newtonsoft.Json.Linq.JArray:0127E335-7E9D-41DC-B272-88D82BD2518F</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.4">
@@ -6536,7 +6477,7 @@
     <row r="31" spans="4:8" x14ac:dyDescent="0.4">
       <c r="E31" t="str">
         <f ca="1">E11</f>
-        <v>Newtonsoft.Json.Linq.JArray:0B767DCE-91EC-45C5-BEE4-8D4A786BC76A</v>
+        <v>Newtonsoft.Json.Linq.JArray:89167A74-51DD-46E6-8B70-EE7D5A78C151</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.4">

</xml_diff>